<commit_message>
asset lijst idee toegevoegd
</commit_message>
<xml_diff>
--- a/Periode 3 game.xlsx
+++ b/Periode 3 game.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfbui\School\Github\periode_3_ontwikkeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382451B2-9551-4403-B4B9-F8348E39FD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42024E6-A5F5-4801-88C9-0FE71FF588C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5ABC62D3-2F78-4A60-908A-30A85BA6A446}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="69">
   <si>
     <t>Game periode 3</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>muur bocht</t>
+  </si>
+  <si>
+    <t>grond stenen toevoeging</t>
   </si>
 </sst>
 </file>
@@ -459,6 +462,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -471,18 +483,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -490,9 +496,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -832,18 +835,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627CB533-94A1-48F6-A962-FD2721E78A03}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
       <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -851,11 +854,11 @@
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
       <c r="D2" s="39"/>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="25"/>
-      <c r="L2" s="26"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="29"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="40"/>
@@ -898,10 +901,10 @@
       <c r="A6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="35"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
@@ -911,10 +914,10 @@
       <c r="G6" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="H6" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="33"/>
+      <c r="I6" s="34"/>
       <c r="J6" t="s">
         <v>3</v>
       </c>
@@ -924,10 +927,10 @@
       <c r="M6" t="s">
         <v>1</v>
       </c>
-      <c r="N6" s="33" t="s">
+      <c r="N6" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="O6" s="33"/>
+      <c r="O6" s="34"/>
       <c r="P6" t="s">
         <v>3</v>
       </c>
@@ -974,11 +977,11 @@
       <c r="N8" t="s">
         <v>36</v>
       </c>
-      <c r="S8" s="30" t="s">
+      <c r="S8" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="T8" s="31"/>
-      <c r="U8" s="32"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="33"/>
     </row>
     <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
@@ -997,11 +1000,11 @@
       <c r="N9" t="s">
         <v>37</v>
       </c>
-      <c r="S9" s="27" t="s">
+      <c r="S9" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="T9" s="28"/>
-      <c r="U9" s="29"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="31"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -1219,20 +1222,28 @@
       <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="13"/>
+      <c r="A23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="23"/>
+      <c r="D23" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="28"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="17" t="s">
         <v>11</v>
       </c>
@@ -1245,10 +1256,10 @@
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="35"/>
+      <c r="C27" s="26"/>
       <c r="D27" s="2" t="s">
         <v>3</v>
       </c>
@@ -1357,10 +1368,10 @@
       <c r="A35" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="28"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="21" t="s">
         <v>13</v>
       </c>
@@ -1373,10 +1384,10 @@
       <c r="A38" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="31"/>
+      <c r="C38" s="25"/>
       <c r="D38" s="22" t="s">
         <v>3</v>
       </c>
@@ -1485,10 +1496,10 @@
       <c r="A46" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B46" s="28" t="s">
+      <c r="B46" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="28"/>
+      <c r="C46" s="24"/>
       <c r="D46" s="17" t="s">
         <v>11</v>
       </c>
@@ -1497,7 +1508,31 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="39">
+  <mergeCells count="40">
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B23:C23"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B32:C32"/>
@@ -1514,29 +1549,6 @@
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="A1:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N12:O12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
dingen toegevoegd aan excel
</commit_message>
<xml_diff>
--- a/Periode 3 game.xlsx
+++ b/Periode 3 game.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/41c270d4a05520e7/Documenten/GitHub/periode_3_ontwikkeling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\GitHub\periode_3_ontwikkeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{FA8E40C5-1819-4317-A621-418B932E5ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{787EEF30-D8DC-4DCA-AD9A-BEE4CDA9E217}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A00860-0289-4410-86B1-5F5509CA5717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5ABC62D3-2F78-4A60-908A-30A85BA6A446}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="83">
   <si>
     <t>Game periode 3</t>
   </si>
@@ -267,6 +267,24 @@
   </si>
   <si>
     <t>7 uur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             brug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       lantaarnpaal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     staande boom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     grotere stenen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        kampvuur</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> stronken als stoelen</t>
   </si>
 </sst>
 </file>
@@ -520,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -543,74 +561,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -621,6 +573,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -938,24 +958,24 @@
   <dimension ref="A1:U46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="49"/>
     </row>
     <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="33"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="52"/>
       <c r="J2" s="39" t="s">
         <v>37</v>
       </c>
@@ -963,10 +983,10 @@
       <c r="L2" s="41"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="36"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="38"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="55"/>
       <c r="S3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1003,10 +1023,10 @@
       <c r="A6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="31"/>
+      <c r="C6" s="42"/>
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1016,10 +1036,10 @@
       <c r="G6" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="29" t="s">
+      <c r="H6" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="I6" s="29"/>
+      <c r="I6" s="47"/>
       <c r="J6" t="s">
         <v>3</v>
       </c>
@@ -1029,10 +1049,10 @@
       <c r="M6" t="s">
         <v>1</v>
       </c>
-      <c r="N6" s="29" t="s">
+      <c r="N6" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="O6" s="29"/>
+      <c r="O6" s="47"/>
       <c r="P6" t="s">
         <v>3</v>
       </c>
@@ -1060,108 +1080,108 @@
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="46" t="s">
+      <c r="G8" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="45" t="s">
+      <c r="H8" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="45"/>
-      <c r="J8" s="48" t="s">
+      <c r="I8" s="35"/>
+      <c r="J8" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="K8" s="47" t="s">
+      <c r="K8" s="25" t="s">
         <v>47</v>
       </c>
       <c r="N8" t="s">
         <v>35</v>
       </c>
-      <c r="S8" s="26" t="s">
+      <c r="S8" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="T8" s="27"/>
-      <c r="U8" s="28"/>
+      <c r="T8" s="38"/>
+      <c r="U8" s="46"/>
     </row>
     <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="22"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="49" t="s">
+      <c r="G9" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="43" t="s">
+      <c r="H9" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="I9" s="43"/>
-      <c r="J9" s="50" t="s">
+      <c r="I9" s="36"/>
+      <c r="J9" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="K9" s="52" t="s">
+      <c r="K9" s="30" t="s">
         <v>76</v>
       </c>
       <c r="N9" t="s">
         <v>36</v>
       </c>
-      <c r="S9" s="23" t="s">
+      <c r="S9" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="T9" s="24"/>
-      <c r="U9" s="25"/>
+      <c r="T9" s="37"/>
+      <c r="U9" s="44"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="51" t="s">
+      <c r="G10" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="43" t="s">
+      <c r="H10" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="I10" s="43"/>
-      <c r="J10" s="50" t="s">
+      <c r="I10" s="36"/>
+      <c r="J10" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="K10" s="52" t="s">
+      <c r="K10" s="30" t="s">
         <v>76</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N10" s="22" t="s">
+      <c r="N10" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="O10" s="22"/>
+      <c r="O10" s="34"/>
       <c r="P10" s="15" t="s">
         <v>12</v>
       </c>
@@ -1173,36 +1193,36 @@
       <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="22"/>
+      <c r="C11" s="34"/>
       <c r="D11" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="51" t="s">
+      <c r="G11" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="43" t="s">
+      <c r="H11" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="I11" s="43"/>
-      <c r="J11" s="54" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="53" t="s">
+      <c r="I11" s="36"/>
+      <c r="J11" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="31" t="s">
         <v>76</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N11" s="22" t="s">
+      <c r="N11" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="O11" s="22"/>
+      <c r="O11" s="34"/>
       <c r="P11" s="17" t="s">
         <v>11</v>
       </c>
@@ -1214,36 +1234,36 @@
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="22"/>
+      <c r="C12" s="34"/>
       <c r="D12" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="51" t="s">
+      <c r="G12" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="43" t="s">
+      <c r="H12" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="I12" s="43"/>
-      <c r="J12" s="54" t="s">
+      <c r="I12" s="36"/>
+      <c r="J12" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="K12" s="52" t="s">
+      <c r="K12" s="30" t="s">
         <v>76</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N12" s="22" t="s">
+      <c r="N12" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="O12" s="22"/>
+      <c r="O12" s="34"/>
       <c r="P12" s="17" t="s">
         <v>11</v>
       </c>
@@ -1255,28 +1275,28 @@
       <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="22"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="55"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
       <c r="M13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N13" s="22" t="s">
+      <c r="N13" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="O13" s="22"/>
+      <c r="O13" s="34"/>
       <c r="P13" s="17" t="s">
         <v>11</v>
       </c>
@@ -1288,86 +1308,115 @@
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="22"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>34</v>
+      </c>
+      <c r="N14" t="s">
+        <v>77</v>
+      </c>
+      <c r="P14" s="57" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="22"/>
+      <c r="C15" s="34"/>
       <c r="D15" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>33</v>
+      </c>
+      <c r="N15" t="s">
+        <v>78</v>
+      </c>
+      <c r="P15" s="15" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="22"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N16" t="s">
+        <v>79</v>
+      </c>
+      <c r="P16" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="22"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N17" t="s">
+        <v>80</v>
+      </c>
+      <c r="P17" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="22"/>
+      <c r="C18" s="34"/>
       <c r="D18" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="N18" s="5"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N18" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="P18" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="22"/>
+      <c r="C19" s="34"/>
       <c r="D19" s="15" t="s">
         <v>12</v>
       </c>
@@ -1375,15 +1424,21 @@
         <v>61</v>
       </c>
       <c r="M19" s="5"/>
-    </row>
-    <row r="20" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N19" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="P19" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="24"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="16" t="s">
         <v>11</v>
       </c>
@@ -1391,15 +1446,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="31"/>
+      <c r="C23" s="42"/>
       <c r="D23" s="2" t="s">
         <v>3</v>
       </c>
@@ -1407,21 +1462,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="13"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="22"/>
+      <c r="C25" s="34"/>
       <c r="D25" s="17" t="s">
         <v>11</v>
       </c>
@@ -1429,14 +1484,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="22"/>
+      <c r="C26" s="34"/>
       <c r="D26" s="17" t="s">
         <v>11</v>
       </c>
@@ -1444,14 +1499,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="22"/>
+      <c r="C27" s="34"/>
       <c r="D27" s="18" t="s">
         <v>10</v>
       </c>
@@ -1459,14 +1514,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="22"/>
+      <c r="C28" s="34"/>
       <c r="D28" s="19" t="s">
         <v>13</v>
       </c>
@@ -1474,14 +1529,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="22"/>
+      <c r="C29" s="34"/>
       <c r="D29" s="19" t="s">
         <v>13</v>
       </c>
@@ -1489,14 +1544,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="22"/>
+      <c r="C30" s="34"/>
       <c r="D30" s="19" t="s">
         <v>13</v>
       </c>
@@ -1504,14 +1559,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="24"/>
+      <c r="C31" s="37"/>
       <c r="D31" s="20" t="s">
         <v>13</v>
       </c>
@@ -1524,10 +1579,10 @@
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="27"/>
+      <c r="C34" s="38"/>
       <c r="D34" s="21" t="s">
         <v>3</v>
       </c>
@@ -1546,10 +1601,10 @@
       <c r="A36" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="22"/>
+      <c r="C36" s="34"/>
       <c r="D36" s="18" t="s">
         <v>10</v>
       </c>
@@ -1561,10 +1616,10 @@
       <c r="A37" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="C37" s="22"/>
+      <c r="C37" s="34"/>
       <c r="D37" s="18" t="s">
         <v>10</v>
       </c>
@@ -1576,10 +1631,10 @@
       <c r="A38" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="22"/>
+      <c r="C38" s="34"/>
       <c r="D38" s="17" t="s">
         <v>11</v>
       </c>
@@ -1591,10 +1646,10 @@
       <c r="A39" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C39" s="22"/>
+      <c r="C39" s="34"/>
       <c r="D39" s="17" t="s">
         <v>11</v>
       </c>
@@ -1606,10 +1661,10 @@
       <c r="A40" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="22"/>
+      <c r="C40" s="34"/>
       <c r="D40" s="18" t="s">
         <v>10</v>
       </c>
@@ -1621,10 +1676,10 @@
       <c r="A41" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="22"/>
+      <c r="C41" s="34"/>
       <c r="D41" s="17" t="s">
         <v>11</v>
       </c>
@@ -1636,10 +1691,10 @@
       <c r="A42" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="24" t="s">
+      <c r="B42" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C42" s="24"/>
+      <c r="C42" s="37"/>
       <c r="D42" s="16" t="s">
         <v>11</v>
       </c>
@@ -1649,9 +1704,9 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="42"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="22"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
     </row>
@@ -1673,6 +1728,37 @@
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="H9:I9"/>
@@ -1689,37 +1775,6 @@
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="A1:D3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N12:O12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
asset list gun toegevoegd
</commit_message>
<xml_diff>
--- a/Periode 3 game.xlsx
+++ b/Periode 3 game.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\GitHub\periode_3_ontwikkeling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfbui\School\Github\periode_3_ontwikkeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3B65F4-EF9B-47D7-84AA-56724854D302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07376936-6BC3-4AC9-B5A6-DED749644FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{5ABC62D3-2F78-4A60-908A-30A85BA6A446}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5ABC62D3-2F78-4A60-908A-30A85BA6A446}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="123">
   <si>
     <t>Game periode 3</t>
   </si>
@@ -381,6 +381,30 @@
   </si>
   <si>
     <t>Gun</t>
+  </si>
+  <si>
+    <t>Gun model</t>
+  </si>
+  <si>
+    <t>Gun UV</t>
+  </si>
+  <si>
+    <t>Gun texture</t>
+  </si>
+  <si>
+    <t>Gun schiet geluid</t>
+  </si>
+  <si>
+    <t>Gun reload geluid</t>
+  </si>
+  <si>
+    <t>Gun reload animatie</t>
+  </si>
+  <si>
+    <t>Gun shoot animatie</t>
+  </si>
+  <si>
+    <t>Gun shoot particles</t>
   </si>
 </sst>
 </file>
@@ -592,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -620,30 +644,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -676,25 +714,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1011,36 +1032,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627CB533-94A1-48F6-A962-FD2721E78A03}">
   <dimension ref="A1:Z107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J71" sqref="J71"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="45"/>
     </row>
     <row r="2" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="44"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="46"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="48"/>
     </row>
     <row r="3" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="47"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="49"/>
-      <c r="J3" s="50" t="s">
+      <c r="A3" s="49"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="51"/>
+      <c r="J3" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="51"/>
-      <c r="L3" s="52"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="54"/>
       <c r="T3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1077,10 +1098,10 @@
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="42"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1090,10 +1111,10 @@
       <c r="G6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="42" t="s">
+      <c r="H6" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="I6" s="42"/>
+      <c r="I6" s="38"/>
       <c r="J6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1103,8 +1124,8 @@
       <c r="M6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
       <c r="P6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1142,10 +1163,10 @@
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="38"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="16" t="s">
         <v>10</v>
       </c>
@@ -1155,10 +1176,10 @@
       <c r="G8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="38" t="s">
+      <c r="H8" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="38"/>
+      <c r="I8" s="34"/>
       <c r="J8" s="25" t="s">
         <v>10</v>
       </c>
@@ -1168,30 +1189,30 @@
       <c r="M8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N8" s="38" t="s">
+      <c r="N8" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="O8" s="38"/>
+      <c r="O8" s="34"/>
       <c r="P8" s="16" t="s">
         <v>10</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="T8" s="55" t="s">
+      <c r="T8" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="U8" s="40"/>
-      <c r="V8" s="56"/>
+      <c r="U8" s="39"/>
+      <c r="V8" s="43"/>
     </row>
     <row r="9" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="38"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="16" t="s">
         <v>10</v>
       </c>
@@ -1201,10 +1222,10 @@
       <c r="G9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="38" t="s">
+      <c r="H9" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="I9" s="38"/>
+      <c r="I9" s="34"/>
       <c r="J9" s="25" t="s">
         <v>10</v>
       </c>
@@ -1214,30 +1235,30 @@
       <c r="M9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N9" s="38" t="s">
+      <c r="N9" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="O9" s="38"/>
+      <c r="O9" s="34"/>
       <c r="P9" s="16" t="s">
         <v>10</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="T9" s="53" t="s">
+      <c r="T9" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="U9" s="39"/>
-      <c r="V9" s="54"/>
+      <c r="U9" s="37"/>
+      <c r="V9" s="41"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="38"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="16" t="s">
         <v>10</v>
       </c>
@@ -1247,10 +1268,10 @@
       <c r="G10" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="38" t="s">
+      <c r="H10" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I10" s="38"/>
+      <c r="I10" s="34"/>
       <c r="J10" s="25" t="s">
         <v>10</v>
       </c>
@@ -1260,10 +1281,10 @@
       <c r="M10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N10" s="38" t="s">
+      <c r="N10" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="O10" s="38"/>
+      <c r="O10" s="34"/>
       <c r="P10" s="16" t="s">
         <v>10</v>
       </c>
@@ -1275,10 +1296,10 @@
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="38"/>
+      <c r="C11" s="34"/>
       <c r="D11" s="16" t="s">
         <v>10</v>
       </c>
@@ -1288,10 +1309,10 @@
       <c r="G11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="38" t="s">
+      <c r="H11" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="I11" s="38"/>
+      <c r="I11" s="34"/>
       <c r="J11" s="25" t="s">
         <v>10</v>
       </c>
@@ -1301,10 +1322,10 @@
       <c r="M11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N11" s="38" t="s">
+      <c r="N11" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="O11" s="38"/>
+      <c r="O11" s="34"/>
       <c r="P11" s="16" t="s">
         <v>10</v>
       </c>
@@ -1316,10 +1337,10 @@
       <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="38"/>
+      <c r="C12" s="34"/>
       <c r="D12" s="16" t="s">
         <v>10</v>
       </c>
@@ -1329,10 +1350,10 @@
       <c r="G12" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="38" t="s">
+      <c r="H12" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="I12" s="38"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="25" t="s">
         <v>10</v>
       </c>
@@ -1342,10 +1363,10 @@
       <c r="M12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N12" s="38" t="s">
+      <c r="N12" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="O12" s="38"/>
+      <c r="O12" s="34"/>
       <c r="P12" s="16" t="s">
         <v>10</v>
       </c>
@@ -1357,10 +1378,10 @@
       <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="38"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="16" t="s">
         <v>10</v>
       </c>
@@ -1370,10 +1391,10 @@
       <c r="G13" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="38" t="s">
+      <c r="H13" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="I13" s="38"/>
+      <c r="I13" s="34"/>
       <c r="J13" s="25" t="s">
         <v>10</v>
       </c>
@@ -1383,10 +1404,10 @@
       <c r="M13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N13" s="38" t="s">
+      <c r="N13" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="O13" s="38"/>
+      <c r="O13" s="34"/>
       <c r="P13" s="16" t="s">
         <v>10</v>
       </c>
@@ -1398,10 +1419,10 @@
       <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="38"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="16" t="s">
         <v>10</v>
       </c>
@@ -1411,10 +1432,10 @@
       <c r="G14" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H14" s="38" t="s">
+      <c r="H14" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="I14" s="38"/>
+      <c r="I14" s="34"/>
       <c r="J14" s="25" t="s">
         <v>10</v>
       </c>
@@ -1424,10 +1445,10 @@
       <c r="M14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N14" s="38" t="s">
+      <c r="N14" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="O14" s="38"/>
+      <c r="O14" s="34"/>
       <c r="P14" s="16" t="s">
         <v>10</v>
       </c>
@@ -1439,10 +1460,10 @@
       <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="38"/>
+      <c r="C15" s="34"/>
       <c r="D15" s="16" t="s">
         <v>10</v>
       </c>
@@ -1452,10 +1473,10 @@
       <c r="G15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H15" s="38" t="s">
+      <c r="H15" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="I15" s="38"/>
+      <c r="I15" s="34"/>
       <c r="J15" s="25" t="s">
         <v>10</v>
       </c>
@@ -1465,10 +1486,10 @@
       <c r="M15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N15" s="38" t="s">
+      <c r="N15" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="O15" s="38"/>
+      <c r="O15" s="34"/>
       <c r="P15" s="16" t="s">
         <v>10</v>
       </c>
@@ -1480,10 +1501,10 @@
       <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="38"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="16" t="s">
         <v>10</v>
       </c>
@@ -1493,10 +1514,10 @@
       <c r="G16" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="38" t="s">
+      <c r="H16" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="I16" s="38"/>
+      <c r="I16" s="34"/>
       <c r="J16" s="26" t="s">
         <v>10</v>
       </c>
@@ -1506,10 +1527,10 @@
       <c r="M16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N16" s="38" t="s">
+      <c r="N16" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="O16" s="38"/>
+      <c r="O16" s="34"/>
       <c r="P16" s="16" t="s">
         <v>10</v>
       </c>
@@ -1521,10 +1542,10 @@
       <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="38"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="16" t="s">
         <v>10</v>
       </c>
@@ -1534,10 +1555,10 @@
       <c r="G17" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H17" s="38" t="s">
+      <c r="H17" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="I17" s="38"/>
+      <c r="I17" s="34"/>
       <c r="J17" s="26" t="s">
         <v>10</v>
       </c>
@@ -1547,10 +1568,10 @@
       <c r="M17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N17" s="38" t="s">
+      <c r="N17" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="O17" s="38"/>
+      <c r="O17" s="34"/>
       <c r="P17" s="16" t="s">
         <v>10</v>
       </c>
@@ -1562,10 +1583,10 @@
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="38"/>
+      <c r="C18" s="34"/>
       <c r="D18" s="16" t="s">
         <v>10</v>
       </c>
@@ -1575,10 +1596,10 @@
       <c r="G18" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H18" s="38" t="s">
+      <c r="H18" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="I18" s="38"/>
+      <c r="I18" s="34"/>
       <c r="J18" s="14" t="s">
         <v>11</v>
       </c>
@@ -1588,10 +1609,10 @@
       <c r="M18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N18" s="38" t="s">
+      <c r="N18" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="O18" s="38"/>
+      <c r="O18" s="34"/>
       <c r="P18" s="16" t="s">
         <v>10</v>
       </c>
@@ -1603,10 +1624,10 @@
       <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="38"/>
+      <c r="C19" s="34"/>
       <c r="D19" s="16" t="s">
         <v>10</v>
       </c>
@@ -1616,10 +1637,10 @@
       <c r="G19" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H19" s="38" t="s">
+      <c r="H19" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="I19" s="38"/>
+      <c r="I19" s="34"/>
       <c r="J19" s="14" t="s">
         <v>11</v>
       </c>
@@ -1629,10 +1650,10 @@
       <c r="M19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N19" s="38" t="s">
+      <c r="N19" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="O19" s="38"/>
+      <c r="O19" s="34"/>
       <c r="P19" s="16" t="s">
         <v>10</v>
       </c>
@@ -1644,10 +1665,10 @@
       <c r="A20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="38"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="16" t="s">
         <v>10</v>
       </c>
@@ -1657,10 +1678,10 @@
       <c r="G20" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="I20" s="38"/>
+      <c r="I20" s="34"/>
       <c r="J20" s="18" t="s">
         <v>12</v>
       </c>
@@ -1670,10 +1691,10 @@
       <c r="M20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N20" s="38" t="s">
+      <c r="N20" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="O20" s="38"/>
+      <c r="O20" s="34"/>
       <c r="P20" s="16" t="s">
         <v>10</v>
       </c>
@@ -1685,10 +1706,10 @@
       <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="38"/>
+      <c r="C21" s="34"/>
       <c r="D21" s="16" t="s">
         <v>10</v>
       </c>
@@ -1698,10 +1719,10 @@
       <c r="G21" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H21" s="38" t="s">
+      <c r="H21" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="I21" s="38"/>
+      <c r="I21" s="34"/>
       <c r="J21" s="18" t="s">
         <v>12</v>
       </c>
@@ -1711,10 +1732,10 @@
       <c r="M21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N21" s="38" t="s">
+      <c r="N21" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="O21" s="38"/>
+      <c r="O21" s="34"/>
       <c r="P21" s="16" t="s">
         <v>10</v>
       </c>
@@ -1726,10 +1747,10 @@
       <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="38"/>
+      <c r="C22" s="34"/>
       <c r="D22" s="16" t="s">
         <v>10</v>
       </c>
@@ -1739,10 +1760,10 @@
       <c r="G22" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H22" s="38" t="s">
+      <c r="H22" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="I22" s="38"/>
+      <c r="I22" s="34"/>
       <c r="J22" s="18" t="s">
         <v>12</v>
       </c>
@@ -1752,10 +1773,10 @@
       <c r="M22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N22" s="38" t="s">
+      <c r="N22" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="O22" s="38"/>
+      <c r="O22" s="34"/>
       <c r="P22" s="16" t="s">
         <v>10</v>
       </c>
@@ -1767,10 +1788,10 @@
       <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="38"/>
+      <c r="C23" s="34"/>
       <c r="D23" s="16" t="s">
         <v>10</v>
       </c>
@@ -1780,10 +1801,10 @@
       <c r="G23" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H23" s="38" t="s">
+      <c r="H23" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="I23" s="38"/>
+      <c r="I23" s="34"/>
       <c r="J23" s="18" t="s">
         <v>12</v>
       </c>
@@ -1793,28 +1814,28 @@
       <c r="M23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N23" s="57" t="s">
+      <c r="N23" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="O23" s="57"/>
+      <c r="O23" s="35"/>
       <c r="P23" s="16" t="s">
         <v>10</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="X23" s="31"/>
-      <c r="Y23" s="30"/>
+      <c r="X23" s="28"/>
+      <c r="Y23" s="27"/>
       <c r="Z23" s="5"/>
     </row>
     <row r="24" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="38"/>
+      <c r="C24" s="34"/>
       <c r="D24" s="16" t="s">
         <v>10</v>
       </c>
@@ -1824,10 +1845,10 @@
       <c r="G24" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="H24" s="39" t="s">
+      <c r="H24" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="I24" s="39"/>
+      <c r="I24" s="37"/>
       <c r="J24" s="19" t="s">
         <v>12</v>
       </c>
@@ -1837,10 +1858,10 @@
       <c r="M24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N24" s="57" t="s">
+      <c r="N24" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="O24" s="57"/>
+      <c r="O24" s="35"/>
       <c r="P24" s="16" t="s">
         <v>10</v>
       </c>
@@ -1848,19 +1869,19 @@
         <v>50</v>
       </c>
       <c r="V24" s="5"/>
-      <c r="W24" s="31"/>
-      <c r="X24" s="31"/>
-      <c r="Y24" s="30"/>
+      <c r="W24" s="28"/>
+      <c r="X24" s="28"/>
+      <c r="Y24" s="27"/>
       <c r="Z24" s="5"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="38" t="s">
+      <c r="B25" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="38"/>
+      <c r="C25" s="34"/>
       <c r="D25" s="16" t="s">
         <v>10</v>
       </c>
@@ -1870,10 +1891,10 @@
       <c r="M25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N25" s="57" t="s">
+      <c r="N25" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="O25" s="57"/>
+      <c r="O25" s="35"/>
       <c r="P25" s="16" t="s">
         <v>10</v>
       </c>
@@ -1885,10 +1906,10 @@
       <c r="A26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="38"/>
+      <c r="C26" s="34"/>
       <c r="D26" s="16" t="s">
         <v>10</v>
       </c>
@@ -1898,10 +1919,10 @@
       <c r="M26" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N26" s="57" t="s">
+      <c r="N26" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="O26" s="57"/>
+      <c r="O26" s="35"/>
       <c r="P26" s="16" t="s">
         <v>10</v>
       </c>
@@ -1913,10 +1934,10 @@
       <c r="A27" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="38"/>
+      <c r="C27" s="34"/>
       <c r="D27" s="16" t="s">
         <v>10</v>
       </c>
@@ -1926,10 +1947,10 @@
       <c r="G27" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H27" s="42" t="s">
+      <c r="H27" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="I27" s="42"/>
+      <c r="I27" s="38"/>
       <c r="J27" s="2" t="s">
         <v>2</v>
       </c>
@@ -1939,10 +1960,10 @@
       <c r="M27" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N27" s="57" t="s">
+      <c r="N27" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="O27" s="57"/>
+      <c r="O27" s="35"/>
       <c r="P27" s="16" t="s">
         <v>10</v>
       </c>
@@ -1954,10 +1975,10 @@
       <c r="A28" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="38"/>
+      <c r="C28" s="34"/>
       <c r="D28" s="16" t="s">
         <v>10</v>
       </c>
@@ -1972,10 +1993,10 @@
       <c r="M28" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N28" s="57" t="s">
+      <c r="N28" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="O28" s="57"/>
+      <c r="O28" s="35"/>
       <c r="P28" s="16" t="s">
         <v>10</v>
       </c>
@@ -1987,10 +2008,10 @@
       <c r="A29" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="38" t="s">
+      <c r="B29" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="38"/>
+      <c r="C29" s="34"/>
       <c r="D29" s="16" t="s">
         <v>10</v>
       </c>
@@ -2000,11 +2021,11 @@
       <c r="G29" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H29" s="38" t="s">
+      <c r="H29" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="I29" s="38"/>
-      <c r="J29" s="27" t="s">
+      <c r="I29" s="34"/>
+      <c r="J29" s="17" t="s">
         <v>9</v>
       </c>
       <c r="K29" s="23" t="s">
@@ -2013,10 +2034,10 @@
       <c r="M29" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N29" s="38" t="s">
+      <c r="N29" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="O29" s="38"/>
+      <c r="O29" s="34"/>
       <c r="P29" s="16" t="s">
         <v>10</v>
       </c>
@@ -2028,10 +2049,10 @@
       <c r="A30" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="38"/>
+      <c r="C30" s="34"/>
       <c r="D30" s="16" t="s">
         <v>10</v>
       </c>
@@ -2041,11 +2062,11 @@
       <c r="G30" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H30" s="38" t="s">
+      <c r="H30" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="I30" s="38"/>
-      <c r="J30" s="27" t="s">
+      <c r="I30" s="34"/>
+      <c r="J30" s="17" t="s">
         <v>9</v>
       </c>
       <c r="K30" s="23" t="s">
@@ -2054,10 +2075,10 @@
       <c r="M30" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N30" s="38" t="s">
+      <c r="N30" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="O30" s="38"/>
+      <c r="O30" s="34"/>
       <c r="P30" s="16" t="s">
         <v>10</v>
       </c>
@@ -2070,10 +2091,10 @@
       <c r="A31" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="38"/>
+      <c r="C31" s="34"/>
       <c r="D31" s="16" t="s">
         <v>10</v>
       </c>
@@ -2083,11 +2104,11 @@
       <c r="G31" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="H31" s="38" t="s">
+      <c r="H31" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="I31" s="38"/>
-      <c r="J31" s="27" t="s">
+      <c r="I31" s="34"/>
+      <c r="J31" s="17" t="s">
         <v>9</v>
       </c>
       <c r="K31" s="23" t="s">
@@ -2096,10 +2117,10 @@
       <c r="M31" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N31" s="38" t="s">
+      <c r="N31" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="O31" s="38"/>
+      <c r="O31" s="34"/>
       <c r="P31" s="16" t="s">
         <v>10</v>
       </c>
@@ -2111,10 +2132,10 @@
       <c r="A32" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="38"/>
+      <c r="C32" s="34"/>
       <c r="D32" s="16" t="s">
         <v>10</v>
       </c>
@@ -2124,11 +2145,11 @@
       <c r="G32" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H32" s="38" t="s">
+      <c r="H32" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="I32" s="38"/>
-      <c r="J32" s="27" t="s">
+      <c r="I32" s="34"/>
+      <c r="J32" s="17" t="s">
         <v>9</v>
       </c>
       <c r="K32" s="23" t="s">
@@ -2137,10 +2158,10 @@
       <c r="M32" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N32" s="38" t="s">
+      <c r="N32" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="O32" s="38"/>
+      <c r="O32" s="34"/>
       <c r="P32" s="14" t="s">
         <v>11</v>
       </c>
@@ -2152,24 +2173,24 @@
       <c r="A33" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="38"/>
+      <c r="C33" s="34"/>
       <c r="D33" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G33" s="35" t="s">
+      <c r="G33" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="H33" s="39" t="s">
+      <c r="H33" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="I33" s="39"/>
-      <c r="J33" s="36" t="s">
+      <c r="I33" s="37"/>
+      <c r="J33" s="56" t="s">
         <v>9</v>
       </c>
       <c r="K33" s="13" t="s">
@@ -2178,10 +2199,10 @@
       <c r="M33" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N33" s="38" t="s">
+      <c r="N33" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="O33" s="38"/>
+      <c r="O33" s="34"/>
       <c r="P33" s="14" t="s">
         <v>11</v>
       </c>
@@ -2193,10 +2214,10 @@
       <c r="A34" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="38"/>
+      <c r="C34" s="34"/>
       <c r="D34" s="16" t="s">
         <v>10</v>
       </c>
@@ -2206,10 +2227,10 @@
       <c r="M34" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N34" s="38" t="s">
+      <c r="N34" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="O34" s="38"/>
+      <c r="O34" s="34"/>
       <c r="P34" s="14" t="s">
         <v>11</v>
       </c>
@@ -2217,14 +2238,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="38" t="s">
+      <c r="B35" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="38"/>
+      <c r="C35" s="34"/>
       <c r="D35" s="16" t="s">
         <v>10</v>
       </c>
@@ -2234,10 +2255,10 @@
       <c r="M35" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N35" s="38" t="s">
+      <c r="N35" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="O35" s="38"/>
+      <c r="O35" s="34"/>
       <c r="P35" s="14" t="s">
         <v>11</v>
       </c>
@@ -2249,23 +2270,36 @@
       <c r="A36" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="38" t="s">
+      <c r="B36" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C36" s="38"/>
+      <c r="C36" s="34"/>
       <c r="D36" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E36" s="12" t="s">
         <v>32</v>
       </c>
+      <c r="G36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H36" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I36" s="38"/>
+      <c r="J36" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="K36" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="M36" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N36" s="38" t="s">
+      <c r="N36" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="O36" s="38"/>
+      <c r="O36" s="34"/>
       <c r="P36" s="14" t="s">
         <v>11</v>
       </c>
@@ -2277,23 +2311,28 @@
       <c r="A37" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="38"/>
+      <c r="C37" s="34"/>
       <c r="D37" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E37" s="12" t="s">
         <v>32</v>
       </c>
+      <c r="G37" s="4"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="12"/>
       <c r="M37" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N37" s="38" t="s">
+      <c r="N37" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="O37" s="38"/>
+      <c r="O37" s="34"/>
       <c r="P37" s="14" t="s">
         <v>11</v>
       </c>
@@ -2305,23 +2344,36 @@
       <c r="A38" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="38"/>
+      <c r="C38" s="34"/>
       <c r="D38" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E38" s="12" t="s">
         <v>72</v>
       </c>
+      <c r="G38" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H38" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="I38" s="34"/>
+      <c r="J38" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="K38" s="12" t="s">
+        <v>73</v>
+      </c>
       <c r="M38" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N38" s="38" t="s">
+      <c r="N38" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="O38" s="38"/>
+      <c r="O38" s="34"/>
       <c r="P38" s="14" t="s">
         <v>11</v>
       </c>
@@ -2333,23 +2385,36 @@
       <c r="A39" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="38" t="s">
+      <c r="B39" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="38"/>
+      <c r="C39" s="34"/>
       <c r="D39" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E39" s="12" t="s">
         <v>32</v>
       </c>
+      <c r="G39" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H39" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="I39" s="34"/>
+      <c r="J39" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="K39" s="12" t="s">
+        <v>73</v>
+      </c>
       <c r="M39" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N39" s="38" t="s">
+      <c r="N39" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="O39" s="38"/>
+      <c r="O39" s="34"/>
       <c r="P39" s="14" t="s">
         <v>11</v>
       </c>
@@ -2361,23 +2426,36 @@
       <c r="A40" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="39" t="s">
+      <c r="B40" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="39"/>
+      <c r="C40" s="37"/>
       <c r="D40" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E40" s="13" t="s">
         <v>32</v>
       </c>
+      <c r="G40" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H40" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="I40" s="34"/>
+      <c r="J40" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="K40" s="12" t="s">
+        <v>73</v>
+      </c>
       <c r="M40" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N40" s="38" t="s">
+      <c r="N40" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="O40" s="38"/>
+      <c r="O40" s="34"/>
       <c r="P40" s="14" t="s">
         <v>11</v>
       </c>
@@ -2386,13 +2464,26 @@
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G41" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H41" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="I41" s="34"/>
+      <c r="J41" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="K41" s="12" t="s">
+        <v>73</v>
+      </c>
       <c r="M41" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N41" s="38" t="s">
+      <c r="N41" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="O41" s="38"/>
+      <c r="O41" s="34"/>
       <c r="P41" s="14" t="s">
         <v>11</v>
       </c>
@@ -2401,13 +2492,26 @@
       </c>
     </row>
     <row r="42" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G42" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H42" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="I42" s="34"/>
+      <c r="J42" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="K42" s="12" t="s">
+        <v>73</v>
+      </c>
       <c r="M42" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N42" s="38" t="s">
+      <c r="N42" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="O42" s="38"/>
+      <c r="O42" s="34"/>
       <c r="P42" s="14" t="s">
         <v>11</v>
       </c>
@@ -2419,23 +2523,36 @@
       <c r="A43" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B43" s="42" t="s">
+      <c r="B43" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="42"/>
+      <c r="C43" s="38"/>
       <c r="D43" s="20" t="s">
         <v>2</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>3</v>
       </c>
+      <c r="G43" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H43" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="I43" s="34"/>
+      <c r="J43" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K43" s="12" t="s">
+        <v>73</v>
+      </c>
       <c r="M43" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N43" s="38" t="s">
+      <c r="N43" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="O43" s="38"/>
+      <c r="O43" s="34"/>
       <c r="P43" s="14" t="s">
         <v>11</v>
       </c>
@@ -2445,18 +2562,31 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
-      <c r="B44" s="31"/>
-      <c r="C44" s="31"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
       <c r="D44" s="21"/>
       <c r="E44" s="12"/>
       <c r="F44" s="5"/>
+      <c r="G44" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H44" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="I44" s="34"/>
+      <c r="J44" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K44" s="12" t="s">
+        <v>73</v>
+      </c>
       <c r="M44" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N44" s="57" t="s">
+      <c r="N44" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="O44" s="57"/>
+      <c r="O44" s="35"/>
       <c r="P44" s="14" t="s">
         <v>11</v>
       </c>
@@ -2464,14 +2594,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="38" t="s">
+      <c r="B45" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="C45" s="38"/>
+      <c r="C45" s="34"/>
       <c r="D45" s="16" t="s">
         <v>10</v>
       </c>
@@ -2479,13 +2609,26 @@
         <v>73</v>
       </c>
       <c r="F45" s="5"/>
+      <c r="G45" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H45" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="I45" s="37"/>
+      <c r="J45" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="K45" s="13" t="s">
+        <v>73</v>
+      </c>
       <c r="M45" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N45" s="57" t="s">
+      <c r="N45" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="O45" s="57"/>
+      <c r="O45" s="35"/>
       <c r="P45" s="14" t="s">
         <v>11</v>
       </c>
@@ -2497,10 +2640,10 @@
       <c r="A46" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B46" s="38" t="s">
+      <c r="B46" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="38"/>
+      <c r="C46" s="34"/>
       <c r="D46" s="16" t="s">
         <v>10</v>
       </c>
@@ -2511,10 +2654,10 @@
       <c r="M46" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N46" s="57" t="s">
+      <c r="N46" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="O46" s="57"/>
+      <c r="O46" s="35"/>
       <c r="P46" s="14" t="s">
         <v>11</v>
       </c>
@@ -2526,10 +2669,10 @@
       <c r="A47" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="38" t="s">
+      <c r="B47" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="38"/>
+      <c r="C47" s="34"/>
       <c r="D47" s="16" t="s">
         <v>10</v>
       </c>
@@ -2539,10 +2682,10 @@
       <c r="M47" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N47" s="57" t="s">
+      <c r="N47" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="O47" s="57"/>
+      <c r="O47" s="35"/>
       <c r="P47" s="14" t="s">
         <v>11</v>
       </c>
@@ -2554,10 +2697,10 @@
       <c r="A48" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B48" s="38" t="s">
+      <c r="B48" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="38"/>
+      <c r="C48" s="34"/>
       <c r="D48" s="16" t="s">
         <v>10</v>
       </c>
@@ -2567,10 +2710,10 @@
       <c r="M48" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N48" s="57" t="s">
+      <c r="N48" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="O48" s="57"/>
+      <c r="O48" s="35"/>
       <c r="P48" s="14" t="s">
         <v>11</v>
       </c>
@@ -2582,10 +2725,10 @@
       <c r="A49" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B49" s="38" t="s">
+      <c r="B49" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="C49" s="38"/>
+      <c r="C49" s="34"/>
       <c r="D49" s="16" t="s">
         <v>10</v>
       </c>
@@ -2595,10 +2738,10 @@
       <c r="M49" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N49" s="57" t="s">
+      <c r="N49" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="O49" s="57"/>
+      <c r="O49" s="35"/>
       <c r="P49" s="14" t="s">
         <v>11</v>
       </c>
@@ -2610,10 +2753,10 @@
       <c r="A50" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B50" s="38" t="s">
+      <c r="B50" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="C50" s="38"/>
+      <c r="C50" s="34"/>
       <c r="D50" s="16" t="s">
         <v>10</v>
       </c>
@@ -2623,10 +2766,10 @@
       <c r="M50" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N50" s="57" t="s">
+      <c r="N50" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="O50" s="57"/>
+      <c r="O50" s="35"/>
       <c r="P50" s="18" t="s">
         <v>12</v>
       </c>
@@ -2638,10 +2781,10 @@
       <c r="A51" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B51" s="38" t="s">
+      <c r="B51" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="C51" s="38"/>
+      <c r="C51" s="34"/>
       <c r="D51" s="16" t="s">
         <v>10</v>
       </c>
@@ -2651,10 +2794,10 @@
       <c r="M51" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N51" s="57" t="s">
+      <c r="N51" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="O51" s="57"/>
+      <c r="O51" s="35"/>
       <c r="P51" s="18" t="s">
         <v>12</v>
       </c>
@@ -2666,10 +2809,10 @@
       <c r="A52" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B52" s="38" t="s">
+      <c r="B52" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="C52" s="38"/>
+      <c r="C52" s="34"/>
       <c r="D52" s="16" t="s">
         <v>10</v>
       </c>
@@ -2679,10 +2822,10 @@
       <c r="M52" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N52" s="57" t="s">
+      <c r="N52" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="O52" s="57"/>
+      <c r="O52" s="35"/>
       <c r="P52" s="18" t="s">
         <v>12</v>
       </c>
@@ -2694,10 +2837,10 @@
       <c r="A53" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B53" s="38" t="s">
+      <c r="B53" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="C53" s="38"/>
+      <c r="C53" s="34"/>
       <c r="D53" s="16" t="s">
         <v>10</v>
       </c>
@@ -2707,10 +2850,10 @@
       <c r="M53" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N53" s="57" t="s">
+      <c r="N53" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="O53" s="57"/>
+      <c r="O53" s="35"/>
       <c r="P53" s="18" t="s">
         <v>12</v>
       </c>
@@ -2722,10 +2865,10 @@
       <c r="A54" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="38" t="s">
+      <c r="B54" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="C54" s="38"/>
+      <c r="C54" s="34"/>
       <c r="D54" s="16" t="s">
         <v>10</v>
       </c>
@@ -2735,10 +2878,10 @@
       <c r="M54" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N54" s="57" t="s">
+      <c r="N54" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="O54" s="57"/>
+      <c r="O54" s="35"/>
       <c r="P54" s="18" t="s">
         <v>12</v>
       </c>
@@ -2750,10 +2893,10 @@
       <c r="A55" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B55" s="38" t="s">
+      <c r="B55" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C55" s="38"/>
+      <c r="C55" s="34"/>
       <c r="D55" s="17" t="s">
         <v>9</v>
       </c>
@@ -2763,10 +2906,10 @@
       <c r="M55" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="N55" s="58" t="s">
+      <c r="N55" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="O55" s="58"/>
+      <c r="O55" s="36"/>
       <c r="P55" s="19" t="s">
         <v>12</v>
       </c>
@@ -2778,10 +2921,10 @@
       <c r="A56" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B56" s="38" t="s">
+      <c r="B56" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="C56" s="38"/>
+      <c r="C56" s="34"/>
       <c r="D56" s="18" t="s">
         <v>12</v>
       </c>
@@ -2793,10 +2936,10 @@
       <c r="A57" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B57" s="38" t="s">
+      <c r="B57" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C57" s="38"/>
+      <c r="C57" s="34"/>
       <c r="D57" s="18" t="s">
         <v>12</v>
       </c>
@@ -2808,10 +2951,10 @@
       <c r="A58" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B58" s="38" t="s">
+      <c r="B58" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C58" s="38"/>
+      <c r="C58" s="34"/>
       <c r="D58" s="18" t="s">
         <v>12</v>
       </c>
@@ -2821,10 +2964,10 @@
       <c r="M58" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N58" s="42" t="s">
+      <c r="N58" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="O58" s="42"/>
+      <c r="O58" s="38"/>
       <c r="P58" s="2" t="s">
         <v>81</v>
       </c>
@@ -2836,10 +2979,10 @@
       <c r="A59" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B59" s="39" t="s">
+      <c r="B59" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="C59" s="39"/>
+      <c r="C59" s="37"/>
       <c r="D59" s="19" t="s">
         <v>12</v>
       </c>
@@ -2856,11 +2999,11 @@
       <c r="M60" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N60" s="38" t="s">
+      <c r="N60" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="O60" s="38"/>
-      <c r="P60" s="27" t="s">
+      <c r="O60" s="34"/>
+      <c r="P60" s="17" t="s">
         <v>9</v>
       </c>
       <c r="Q60" s="12" t="s">
@@ -2871,11 +3014,11 @@
       <c r="M61" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N61" s="38" t="s">
+      <c r="N61" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="O61" s="38"/>
-      <c r="P61" s="27" t="s">
+      <c r="O61" s="34"/>
+      <c r="P61" s="17" t="s">
         <v>9</v>
       </c>
       <c r="Q61" s="12" t="s">
@@ -2886,10 +3029,10 @@
       <c r="A62" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B62" s="40" t="s">
+      <c r="B62" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="C62" s="40"/>
+      <c r="C62" s="39"/>
       <c r="D62" s="20" t="s">
         <v>2</v>
       </c>
@@ -2899,11 +3042,11 @@
       <c r="M62" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N62" s="38" t="s">
+      <c r="N62" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="O62" s="38"/>
-      <c r="P62" s="27" t="s">
+      <c r="O62" s="34"/>
+      <c r="P62" s="17" t="s">
         <v>9</v>
       </c>
       <c r="Q62" s="12" t="s">
@@ -2919,11 +3062,11 @@
       <c r="M63" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N63" s="38" t="s">
+      <c r="N63" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="O63" s="38"/>
-      <c r="P63" s="27" t="s">
+      <c r="O63" s="34"/>
+      <c r="P63" s="17" t="s">
         <v>9</v>
       </c>
       <c r="Q63" s="12" t="s">
@@ -2934,10 +3077,10 @@
       <c r="A64" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B64" s="38" t="s">
+      <c r="B64" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="C64" s="38"/>
+      <c r="C64" s="34"/>
       <c r="D64" s="17" t="s">
         <v>9</v>
       </c>
@@ -2947,11 +3090,11 @@
       <c r="M64" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N64" s="38" t="s">
+      <c r="N64" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="O64" s="38"/>
-      <c r="P64" s="28" t="s">
+      <c r="O64" s="34"/>
+      <c r="P64" s="17" t="s">
         <v>9</v>
       </c>
       <c r="Q64" s="12" t="s">
@@ -2962,10 +3105,10 @@
       <c r="A65" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B65" s="38" t="s">
+      <c r="B65" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="C65" s="38"/>
+      <c r="C65" s="34"/>
       <c r="D65" s="17" t="s">
         <v>9</v>
       </c>
@@ -2975,11 +3118,11 @@
       <c r="M65" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="N65" s="39" t="s">
+      <c r="N65" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="O65" s="39"/>
-      <c r="P65" s="29" t="s">
+      <c r="O65" s="37"/>
+      <c r="P65" s="56" t="s">
         <v>9</v>
       </c>
       <c r="Q65" s="13" t="s">
@@ -2990,10 +3133,10 @@
       <c r="A66" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B66" s="38" t="s">
+      <c r="B66" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="C66" s="38"/>
+      <c r="C66" s="34"/>
       <c r="D66" s="16" t="s">
         <v>10</v>
       </c>
@@ -3005,10 +3148,10 @@
       <c r="A67" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B67" s="38" t="s">
+      <c r="B67" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="C67" s="38"/>
+      <c r="C67" s="34"/>
       <c r="D67" s="16" t="s">
         <v>10</v>
       </c>
@@ -3020,37 +3163,25 @@
       <c r="A68" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B68" s="38" t="s">
+      <c r="B68" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="C68" s="38"/>
+      <c r="C68" s="34"/>
       <c r="D68" s="17" t="s">
         <v>9</v>
       </c>
       <c r="E68" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="M68" t="s">
-        <v>37</v>
-      </c>
-      <c r="N68" t="s">
-        <v>114</v>
-      </c>
-      <c r="P68" s="59" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q68" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B69" s="38" t="s">
+      <c r="B69" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C69" s="38"/>
+      <c r="C69" s="34"/>
       <c r="D69" s="16" t="s">
         <v>10</v>
       </c>
@@ -3062,10 +3193,10 @@
       <c r="A70" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B70" s="39" t="s">
+      <c r="B70" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C70" s="39"/>
+      <c r="C70" s="37"/>
       <c r="D70" s="15" t="s">
         <v>10</v>
       </c>
@@ -3074,19 +3205,19 @@
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A80" s="32"/>
-      <c r="B80" s="33"/>
-      <c r="C80" s="33"/>
+      <c r="A80" s="29"/>
+      <c r="B80" s="30"/>
+      <c r="C80" s="30"/>
       <c r="D80" s="22"/>
       <c r="E80" s="22"/>
       <c r="G80" s="22"/>
-      <c r="H80" s="33"/>
-      <c r="I80" s="33"/>
+      <c r="H80" s="30"/>
+      <c r="I80" s="30"/>
       <c r="J80" s="22"/>
       <c r="K80" s="22"/>
       <c r="M80" s="22"/>
-      <c r="N80" s="33"/>
-      <c r="O80" s="33"/>
+      <c r="N80" s="30"/>
+      <c r="O80" s="30"/>
       <c r="P80" s="22"/>
       <c r="Q80" s="22"/>
     </row>
@@ -3109,189 +3240,189 @@
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" s="22"/>
-      <c r="B82" s="32"/>
-      <c r="C82" s="32"/>
-      <c r="D82" s="30"/>
+      <c r="B82" s="29"/>
+      <c r="C82" s="29"/>
+      <c r="D82" s="27"/>
       <c r="E82" s="22"/>
       <c r="G82" s="22"/>
-      <c r="H82" s="32"/>
-      <c r="I82" s="32"/>
-      <c r="J82" s="30"/>
+      <c r="H82" s="29"/>
+      <c r="I82" s="29"/>
+      <c r="J82" s="27"/>
       <c r="K82" s="22"/>
       <c r="M82" s="22"/>
-      <c r="N82" s="32"/>
-      <c r="O82" s="32"/>
-      <c r="P82" s="30"/>
+      <c r="N82" s="29"/>
+      <c r="O82" s="29"/>
+      <c r="P82" s="27"/>
       <c r="Q82" s="22"/>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" s="22"/>
-      <c r="B83" s="32"/>
-      <c r="C83" s="32"/>
-      <c r="D83" s="30"/>
+      <c r="B83" s="29"/>
+      <c r="C83" s="29"/>
+      <c r="D83" s="27"/>
       <c r="E83" s="22"/>
       <c r="G83" s="22"/>
-      <c r="H83" s="32"/>
-      <c r="I83" s="32"/>
-      <c r="J83" s="30"/>
+      <c r="H83" s="29"/>
+      <c r="I83" s="29"/>
+      <c r="J83" s="27"/>
       <c r="K83" s="22"/>
       <c r="M83" s="22"/>
-      <c r="N83" s="32"/>
-      <c r="O83" s="32"/>
-      <c r="P83" s="30"/>
+      <c r="N83" s="29"/>
+      <c r="O83" s="29"/>
+      <c r="P83" s="27"/>
       <c r="Q83" s="22"/>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" s="22"/>
-      <c r="B84" s="32"/>
-      <c r="C84" s="32"/>
-      <c r="D84" s="30"/>
+      <c r="B84" s="29"/>
+      <c r="C84" s="29"/>
+      <c r="D84" s="27"/>
       <c r="E84" s="22"/>
       <c r="G84" s="22"/>
-      <c r="H84" s="32"/>
-      <c r="I84" s="32"/>
-      <c r="J84" s="30"/>
+      <c r="H84" s="29"/>
+      <c r="I84" s="29"/>
+      <c r="J84" s="27"/>
       <c r="K84" s="22"/>
       <c r="M84" s="22"/>
-      <c r="N84" s="32"/>
-      <c r="O84" s="32"/>
-      <c r="P84" s="30"/>
+      <c r="N84" s="29"/>
+      <c r="O84" s="29"/>
+      <c r="P84" s="27"/>
       <c r="Q84" s="22"/>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" s="22"/>
-      <c r="B85" s="32"/>
-      <c r="C85" s="32"/>
-      <c r="D85" s="30"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="27"/>
       <c r="E85" s="22"/>
       <c r="G85" s="22"/>
-      <c r="H85" s="32"/>
-      <c r="I85" s="32"/>
-      <c r="J85" s="34"/>
+      <c r="H85" s="29"/>
+      <c r="I85" s="29"/>
+      <c r="J85" s="31"/>
       <c r="K85" s="22"/>
       <c r="M85" s="22"/>
-      <c r="N85" s="32"/>
-      <c r="O85" s="32"/>
-      <c r="P85" s="30"/>
+      <c r="N85" s="29"/>
+      <c r="O85" s="29"/>
+      <c r="P85" s="27"/>
       <c r="Q85" s="22"/>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" s="22"/>
-      <c r="B86" s="32"/>
-      <c r="C86" s="32"/>
-      <c r="D86" s="30"/>
+      <c r="B86" s="29"/>
+      <c r="C86" s="29"/>
+      <c r="D86" s="27"/>
       <c r="E86" s="22"/>
       <c r="G86" s="22"/>
-      <c r="H86" s="32"/>
-      <c r="I86" s="32"/>
-      <c r="J86" s="30"/>
+      <c r="H86" s="29"/>
+      <c r="I86" s="29"/>
+      <c r="J86" s="27"/>
       <c r="K86" s="22"/>
       <c r="M86" s="22"/>
-      <c r="N86" s="32"/>
-      <c r="O86" s="32"/>
-      <c r="P86" s="30"/>
+      <c r="N86" s="29"/>
+      <c r="O86" s="29"/>
+      <c r="P86" s="27"/>
       <c r="Q86" s="22"/>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87" s="22"/>
-      <c r="B87" s="32"/>
-      <c r="C87" s="32"/>
-      <c r="D87" s="30"/>
+      <c r="B87" s="29"/>
+      <c r="C87" s="29"/>
+      <c r="D87" s="27"/>
       <c r="E87" s="22"/>
       <c r="G87" s="22"/>
-      <c r="H87" s="32"/>
-      <c r="I87" s="32"/>
-      <c r="J87" s="30"/>
+      <c r="H87" s="29"/>
+      <c r="I87" s="29"/>
+      <c r="J87" s="27"/>
       <c r="K87" s="22"/>
       <c r="M87" s="22"/>
-      <c r="N87" s="32"/>
-      <c r="O87" s="32"/>
-      <c r="P87" s="30"/>
+      <c r="N87" s="29"/>
+      <c r="O87" s="29"/>
+      <c r="P87" s="27"/>
       <c r="Q87" s="22"/>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" s="22"/>
-      <c r="B88" s="32"/>
-      <c r="C88" s="32"/>
-      <c r="D88" s="30"/>
+      <c r="B88" s="29"/>
+      <c r="C88" s="29"/>
+      <c r="D88" s="27"/>
       <c r="E88" s="22"/>
       <c r="G88" s="22"/>
-      <c r="H88" s="32"/>
-      <c r="I88" s="32"/>
-      <c r="J88" s="30"/>
+      <c r="H88" s="29"/>
+      <c r="I88" s="29"/>
+      <c r="J88" s="27"/>
       <c r="K88" s="22"/>
       <c r="M88" s="22"/>
-      <c r="N88" s="32"/>
-      <c r="O88" s="32"/>
-      <c r="P88" s="30"/>
+      <c r="N88" s="29"/>
+      <c r="O88" s="29"/>
+      <c r="P88" s="27"/>
       <c r="Q88" s="22"/>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89" s="22"/>
-      <c r="B89" s="32"/>
-      <c r="C89" s="32"/>
-      <c r="D89" s="30"/>
+      <c r="B89" s="29"/>
+      <c r="C89" s="29"/>
+      <c r="D89" s="27"/>
       <c r="E89" s="22"/>
       <c r="G89" s="22"/>
-      <c r="H89" s="32"/>
-      <c r="I89" s="32"/>
-      <c r="J89" s="30"/>
+      <c r="H89" s="29"/>
+      <c r="I89" s="29"/>
+      <c r="J89" s="27"/>
       <c r="K89" s="22"/>
       <c r="M89" s="22"/>
-      <c r="N89" s="32"/>
-      <c r="O89" s="32"/>
-      <c r="P89" s="30"/>
+      <c r="N89" s="29"/>
+      <c r="O89" s="29"/>
+      <c r="P89" s="27"/>
       <c r="Q89" s="22"/>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" s="22"/>
-      <c r="B90" s="32"/>
-      <c r="C90" s="32"/>
-      <c r="D90" s="30"/>
+      <c r="B90" s="29"/>
+      <c r="C90" s="29"/>
+      <c r="D90" s="27"/>
       <c r="E90" s="22"/>
       <c r="G90" s="22"/>
-      <c r="H90" s="32"/>
-      <c r="I90" s="32"/>
-      <c r="J90" s="30"/>
+      <c r="H90" s="29"/>
+      <c r="I90" s="29"/>
+      <c r="J90" s="27"/>
       <c r="K90" s="22"/>
       <c r="M90" s="22"/>
-      <c r="N90" s="32"/>
-      <c r="O90" s="32"/>
-      <c r="P90" s="30"/>
+      <c r="N90" s="29"/>
+      <c r="O90" s="29"/>
+      <c r="P90" s="27"/>
       <c r="Q90" s="22"/>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" s="22"/>
-      <c r="B91" s="32"/>
-      <c r="C91" s="32"/>
-      <c r="D91" s="30"/>
+      <c r="B91" s="29"/>
+      <c r="C91" s="29"/>
+      <c r="D91" s="27"/>
       <c r="E91" s="22"/>
       <c r="G91" s="22"/>
-      <c r="H91" s="32"/>
-      <c r="I91" s="32"/>
-      <c r="J91" s="30"/>
+      <c r="H91" s="29"/>
+      <c r="I91" s="29"/>
+      <c r="J91" s="27"/>
       <c r="K91" s="22"/>
       <c r="M91" s="22"/>
-      <c r="N91" s="32"/>
-      <c r="O91" s="32"/>
-      <c r="P91" s="30"/>
+      <c r="N91" s="29"/>
+      <c r="O91" s="29"/>
+      <c r="P91" s="27"/>
       <c r="Q91" s="22"/>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" s="22"/>
-      <c r="B92" s="32"/>
-      <c r="C92" s="32"/>
-      <c r="D92" s="30"/>
+      <c r="B92" s="29"/>
+      <c r="C92" s="29"/>
+      <c r="D92" s="27"/>
       <c r="E92" s="22"/>
       <c r="G92" s="22"/>
-      <c r="H92" s="32"/>
-      <c r="I92" s="32"/>
-      <c r="J92" s="30"/>
+      <c r="H92" s="29"/>
+      <c r="I92" s="29"/>
+      <c r="J92" s="27"/>
       <c r="K92" s="22"/>
       <c r="M92" s="22"/>
-      <c r="N92" s="32"/>
-      <c r="O92" s="32"/>
-      <c r="P92" s="30"/>
+      <c r="N92" s="29"/>
+      <c r="O92" s="29"/>
+      <c r="P92" s="27"/>
       <c r="Q92" s="22"/>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.3">
@@ -3301,14 +3432,14 @@
       <c r="D93" s="22"/>
       <c r="E93" s="22"/>
       <c r="G93" s="22"/>
-      <c r="H93" s="32"/>
-      <c r="I93" s="32"/>
-      <c r="J93" s="30"/>
+      <c r="H93" s="29"/>
+      <c r="I93" s="29"/>
+      <c r="J93" s="27"/>
       <c r="K93" s="22"/>
       <c r="M93" s="22"/>
-      <c r="N93" s="32"/>
-      <c r="O93" s="32"/>
-      <c r="P93" s="30"/>
+      <c r="N93" s="29"/>
+      <c r="O93" s="29"/>
+      <c r="P93" s="27"/>
       <c r="Q93" s="22"/>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.3">
@@ -3318,26 +3449,26 @@
       <c r="D94" s="22"/>
       <c r="E94" s="22"/>
       <c r="G94" s="22"/>
-      <c r="H94" s="32"/>
-      <c r="I94" s="32"/>
-      <c r="J94" s="30"/>
+      <c r="H94" s="29"/>
+      <c r="I94" s="29"/>
+      <c r="J94" s="27"/>
       <c r="K94" s="22"/>
       <c r="M94" s="22"/>
-      <c r="N94" s="32"/>
-      <c r="O94" s="32"/>
-      <c r="P94" s="30"/>
+      <c r="N94" s="29"/>
+      <c r="O94" s="29"/>
+      <c r="P94" s="27"/>
       <c r="Q94" s="22"/>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95" s="22"/>
-      <c r="B95" s="33"/>
-      <c r="C95" s="33"/>
+      <c r="B95" s="30"/>
+      <c r="C95" s="30"/>
       <c r="D95" s="22"/>
       <c r="E95" s="22"/>
       <c r="M95" s="22"/>
-      <c r="N95" s="32"/>
-      <c r="O95" s="32"/>
-      <c r="P95" s="30"/>
+      <c r="N95" s="29"/>
+      <c r="O95" s="29"/>
+      <c r="P95" s="27"/>
       <c r="Q95" s="22"/>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.3">
@@ -3347,35 +3478,35 @@
       <c r="D96" s="22"/>
       <c r="E96" s="22"/>
       <c r="M96" s="22"/>
-      <c r="N96" s="32"/>
-      <c r="O96" s="32"/>
-      <c r="P96" s="30"/>
+      <c r="N96" s="29"/>
+      <c r="O96" s="29"/>
+      <c r="P96" s="27"/>
       <c r="Q96" s="22"/>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97" s="22"/>
-      <c r="B97" s="32"/>
-      <c r="C97" s="32"/>
-      <c r="D97" s="30"/>
+      <c r="B97" s="29"/>
+      <c r="C97" s="29"/>
+      <c r="D97" s="27"/>
       <c r="E97" s="22"/>
       <c r="M97" s="22"/>
-      <c r="N97" s="32"/>
-      <c r="O97" s="32"/>
-      <c r="P97" s="30"/>
+      <c r="N97" s="29"/>
+      <c r="O97" s="29"/>
+      <c r="P97" s="27"/>
       <c r="Q97" s="22"/>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98" s="22"/>
-      <c r="B98" s="32"/>
-      <c r="C98" s="32"/>
-      <c r="D98" s="30"/>
+      <c r="B98" s="29"/>
+      <c r="C98" s="29"/>
+      <c r="D98" s="27"/>
       <c r="E98" s="22"/>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99" s="22"/>
-      <c r="B99" s="32"/>
-      <c r="C99" s="32"/>
-      <c r="D99" s="30"/>
+      <c r="B99" s="29"/>
+      <c r="C99" s="29"/>
+      <c r="D99" s="27"/>
       <c r="E99" s="22"/>
       <c r="F99" s="5"/>
       <c r="G99" s="5"/>
@@ -3386,9 +3517,9 @@
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100" s="22"/>
-      <c r="B100" s="32"/>
-      <c r="C100" s="32"/>
-      <c r="D100" s="30"/>
+      <c r="B100" s="29"/>
+      <c r="C100" s="29"/>
+      <c r="D100" s="27"/>
       <c r="E100" s="22"/>
       <c r="F100" s="5"/>
       <c r="G100" s="5"/>
@@ -3399,9 +3530,9 @@
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101" s="22"/>
-      <c r="B101" s="32"/>
-      <c r="C101" s="32"/>
-      <c r="D101" s="30"/>
+      <c r="B101" s="29"/>
+      <c r="C101" s="29"/>
+      <c r="D101" s="27"/>
       <c r="E101" s="22"/>
       <c r="F101" s="5"/>
       <c r="G101" s="5"/>
@@ -3412,9 +3543,9 @@
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" s="22"/>
-      <c r="B102" s="32"/>
-      <c r="C102" s="32"/>
-      <c r="D102" s="30"/>
+      <c r="B102" s="29"/>
+      <c r="C102" s="29"/>
+      <c r="D102" s="27"/>
       <c r="E102" s="22"/>
       <c r="F102" s="5"/>
       <c r="G102" s="5"/>
@@ -3425,14 +3556,14 @@
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" s="22"/>
-      <c r="B103" s="32"/>
-      <c r="C103" s="32"/>
-      <c r="D103" s="30"/>
+      <c r="B103" s="29"/>
+      <c r="C103" s="29"/>
+      <c r="D103" s="27"/>
       <c r="E103" s="22"/>
       <c r="F103" s="5"/>
       <c r="G103" s="5"/>
-      <c r="H103" s="31"/>
-      <c r="I103" s="31"/>
+      <c r="H103" s="28"/>
+      <c r="I103" s="28"/>
       <c r="J103" s="5"/>
       <c r="K103" s="5"/>
     </row>
@@ -3449,8 +3580,8 @@
       <c r="E105" s="5"/>
       <c r="F105" s="5"/>
       <c r="G105" s="5"/>
-      <c r="H105" s="37"/>
-      <c r="I105" s="37"/>
+      <c r="H105" s="33"/>
+      <c r="I105" s="33"/>
       <c r="J105" s="5"/>
       <c r="K105" s="5"/>
     </row>
@@ -3473,28 +3604,113 @@
       <c r="K107" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="142">
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="N40:O40"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="N42:O42"/>
-    <mergeCell ref="N43:O43"/>
-    <mergeCell ref="N54:O54"/>
-    <mergeCell ref="N55:O55"/>
-    <mergeCell ref="N49:O49"/>
-    <mergeCell ref="N50:O50"/>
-    <mergeCell ref="N51:O51"/>
-    <mergeCell ref="N52:O52"/>
-    <mergeCell ref="N53:O53"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="N46:O46"/>
-    <mergeCell ref="N47:O47"/>
-    <mergeCell ref="N48:O48"/>
+  <mergeCells count="151">
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="T9:V9"/>
+    <mergeCell ref="T8:V8"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="N65:O65"/>
+    <mergeCell ref="N64:O64"/>
+    <mergeCell ref="N63:O63"/>
+    <mergeCell ref="N62:O62"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="N60:O60"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="B39:C39"/>
@@ -3519,103 +3735,27 @@
     <mergeCell ref="B52:C52"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="N58:O58"/>
-    <mergeCell ref="N65:O65"/>
-    <mergeCell ref="N64:O64"/>
-    <mergeCell ref="N63:O63"/>
-    <mergeCell ref="N62:O62"/>
-    <mergeCell ref="N61:O61"/>
-    <mergeCell ref="N60:O60"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="T9:V9"/>
-    <mergeCell ref="T8:V8"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="A1:D3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="N42:O42"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="N54:O54"/>
+    <mergeCell ref="N55:O55"/>
+    <mergeCell ref="N49:O49"/>
+    <mergeCell ref="N50:O50"/>
+    <mergeCell ref="N51:O51"/>
+    <mergeCell ref="N52:O52"/>
+    <mergeCell ref="N53:O53"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="N48:O48"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
wat shit in unity geplaatst
</commit_message>
<xml_diff>
--- a/Periode 3 game.xlsx
+++ b/Periode 3 game.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfbui\School\Github\periode_3_ontwikkeling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\GitHub\periode_3_ontwikkeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DBA116-D7B4-4CE2-A465-9C71B2AAF824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6A430D-BDBA-4DC2-9F14-7B4F33903762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5ABC62D3-2F78-4A60-908A-30A85BA6A446}"/>
   </bookViews>
@@ -778,13 +778,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -793,38 +792,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -836,7 +836,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -860,22 +860,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1184,7 +1169,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1192,38 +1177,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627CB533-94A1-48F6-A962-FD2721E78A03}">
-  <dimension ref="A1:Z107"/>
+  <dimension ref="A1:Y105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17:O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="14" max="14" width="33.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="41"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="42"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="36"/>
     </row>
     <row r="3" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="45"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="47"/>
-      <c r="J3" s="48" t="s">
+      <c r="A3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="39"/>
+      <c r="J3" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="49"/>
-      <c r="L3" s="50"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="42"/>
       <c r="T3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1238,10 +1226,10 @@
       <c r="T4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="U4" s="5" t="s">
+      <c r="U4" t="s">
         <v>8</v>
       </c>
-      <c r="V4" s="6" t="s">
+      <c r="V4" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1249,10 +1237,10 @@
       <c r="T5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="U5" t="s">
         <v>8</v>
       </c>
-      <c r="V5" s="7" t="s">
+      <c r="V5" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1260,197 +1248,188 @@
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="37"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="37"/>
+      <c r="I6" s="26"/>
       <c r="J6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="10" t="s">
         <v>3</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
       <c r="P6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="Q6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="T6" s="8" t="s">
+      <c r="T6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="U6" s="9" t="s">
+      <c r="U6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="V6" s="10" t="s">
+      <c r="V6" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="12"/>
+      <c r="E7" s="11"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="12"/>
+      <c r="K7" s="11"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="12"/>
+      <c r="Q7" s="11"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="12" t="s">
+      <c r="C8" s="24"/>
+      <c r="D8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="I8" s="36"/>
-      <c r="J8" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" s="12" t="s">
+      <c r="I8" s="24"/>
+      <c r="J8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="36" t="s">
+      <c r="N8" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="O8" s="36"/>
-      <c r="P8" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q8" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="T8" s="53" t="s">
+      <c r="O8" s="24"/>
+      <c r="P8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="T8" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="U8" s="39"/>
-      <c r="V8" s="54"/>
+      <c r="U8" s="27"/>
+      <c r="V8" s="31"/>
     </row>
     <row r="9" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="12" t="s">
+      <c r="C9" s="24"/>
+      <c r="D9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="I9" s="36"/>
-      <c r="J9" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="K9" s="12" t="s">
+      <c r="I9" s="24"/>
+      <c r="J9" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N9" s="36" t="s">
+      <c r="N9" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="O9" s="36"/>
-      <c r="P9" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q9" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="T9" s="51" t="s">
+      <c r="O9" s="24"/>
+      <c r="P9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q9" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="T9" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="U9" s="38"/>
-      <c r="V9" s="52"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="29"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="12" t="s">
+      <c r="C10" s="24"/>
+      <c r="D10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="36" t="s">
+      <c r="H10" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="I10" s="36"/>
-      <c r="J10" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" s="12" t="s">
+      <c r="I10" s="24"/>
+      <c r="J10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="36" t="s">
+      <c r="N10" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="O10" s="36"/>
-      <c r="P10" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q10" s="12" t="s">
+      <c r="O10" s="24"/>
+      <c r="P10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q10" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1458,40 +1437,40 @@
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="12" t="s">
+      <c r="C11" s="24"/>
+      <c r="D11" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="36" t="s">
+      <c r="H11" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="I11" s="36"/>
-      <c r="J11" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="12" t="s">
+      <c r="I11" s="24"/>
+      <c r="J11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N11" s="36" t="s">
+      <c r="N11" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="O11" s="36"/>
-      <c r="P11" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q11" s="12" t="s">
+      <c r="O11" s="24"/>
+      <c r="P11" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q11" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1499,40 +1478,40 @@
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="12" t="s">
+      <c r="C12" s="24"/>
+      <c r="D12" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="36" t="s">
+      <c r="H12" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="36"/>
-      <c r="J12" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="12" t="s">
+      <c r="I12" s="24"/>
+      <c r="J12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N12" s="36" t="s">
+      <c r="N12" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="O12" s="36"/>
-      <c r="P12" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q12" s="12" t="s">
+      <c r="O12" s="24"/>
+      <c r="P12" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1540,40 +1519,40 @@
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="12" t="s">
+      <c r="C13" s="24"/>
+      <c r="D13" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="36" t="s">
+      <c r="H13" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="I13" s="36"/>
-      <c r="J13" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="12" t="s">
+      <c r="I13" s="24"/>
+      <c r="J13" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N13" s="36" t="s">
+      <c r="N13" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="O13" s="36"/>
-      <c r="P13" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q13" s="12" t="s">
+      <c r="O13" s="24"/>
+      <c r="P13" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q13" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1581,40 +1560,40 @@
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="12" t="s">
+      <c r="C14" s="24"/>
+      <c r="D14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="36" t="s">
+      <c r="H14" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="I14" s="36"/>
-      <c r="J14" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" s="12" t="s">
+      <c r="I14" s="24"/>
+      <c r="J14" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N14" s="36" t="s">
+      <c r="N14" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="O14" s="36"/>
-      <c r="P14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q14" s="12" t="s">
+      <c r="O14" s="24"/>
+      <c r="P14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1622,40 +1601,40 @@
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="12" t="s">
+      <c r="C15" s="24"/>
+      <c r="D15" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="36" t="s">
+      <c r="H15" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="I15" s="36"/>
-      <c r="J15" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="K15" s="12" t="s">
+      <c r="I15" s="24"/>
+      <c r="J15" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N15" s="36" t="s">
+      <c r="N15" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="O15" s="36"/>
-      <c r="P15" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q15" s="12" t="s">
+      <c r="O15" s="24"/>
+      <c r="P15" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q15" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1663,671 +1642,661 @@
       <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="12" t="s">
+      <c r="C16" s="24"/>
+      <c r="D16" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="36" t="s">
+      <c r="H16" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="I16" s="36"/>
-      <c r="J16" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="K16" s="12" t="s">
+      <c r="I16" s="24"/>
+      <c r="J16" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N16" s="36" t="s">
+      <c r="N16" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="O16" s="36"/>
-      <c r="P16" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q16" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="O16" s="24"/>
+      <c r="P16" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q16" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="12" t="s">
+      <c r="C17" s="24"/>
+      <c r="D17" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="24" t="s">
+      <c r="G17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="36" t="s">
+      <c r="H17" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="I17" s="36"/>
-      <c r="J17" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="K17" s="12" t="s">
+      <c r="I17" s="24"/>
+      <c r="J17" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K17" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N17" s="36" t="s">
+      <c r="N17" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="O17" s="36"/>
-      <c r="P17" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q17" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="O17" s="43"/>
+      <c r="P17" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q17" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="12" t="s">
+      <c r="C18" s="24"/>
+      <c r="D18" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="24" t="s">
+      <c r="G18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H18" s="36" t="s">
+      <c r="H18" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="I18" s="36"/>
-      <c r="J18" s="14" t="s">
+      <c r="I18" s="24"/>
+      <c r="J18" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="K18" s="12" t="s">
+      <c r="K18" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N18" s="36" t="s">
+      <c r="N18" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="O18" s="36"/>
-      <c r="P18" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q18" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="O18" s="43"/>
+      <c r="P18" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="12" t="s">
+      <c r="C19" s="24"/>
+      <c r="D19" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="24" t="s">
+      <c r="G19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H19" s="36" t="s">
+      <c r="H19" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="36"/>
-      <c r="J19" s="14" t="s">
+      <c r="I19" s="24"/>
+      <c r="J19" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="K19" s="12" t="s">
+      <c r="K19" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N19" s="36" t="s">
+      <c r="N19" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="O19" s="36"/>
-      <c r="P19" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q19" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="O19" s="43"/>
+      <c r="P19" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q19" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="12" t="s">
+      <c r="C20" s="24"/>
+      <c r="D20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="24" t="s">
+      <c r="G20" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H20" s="36" t="s">
+      <c r="H20" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="18" t="s">
+      <c r="I20" s="24"/>
+      <c r="J20" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="K20" s="12" t="s">
+      <c r="K20" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N20" s="36" t="s">
+      <c r="N20" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="O20" s="36"/>
-      <c r="P20" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q20" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="O20" s="24"/>
+      <c r="P20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q20" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="12" t="s">
+      <c r="C21" s="24"/>
+      <c r="D21" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="24" t="s">
+      <c r="G21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H21" s="36" t="s">
+      <c r="H21" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="I21" s="36"/>
-      <c r="J21" s="18" t="s">
+      <c r="I21" s="24"/>
+      <c r="J21" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="K21" s="12" t="s">
+      <c r="K21" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N21" s="36" t="s">
+      <c r="N21" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="O21" s="36"/>
-      <c r="P21" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q21" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="O21" s="24"/>
+      <c r="P21" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q21" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="12" t="s">
+      <c r="C22" s="24"/>
+      <c r="D22" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G22" s="24" t="s">
+      <c r="G22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H22" s="36" t="s">
+      <c r="H22" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="I22" s="36"/>
-      <c r="J22" s="18" t="s">
+      <c r="I22" s="24"/>
+      <c r="J22" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="K22" s="12" t="s">
+      <c r="K22" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N22" s="36" t="s">
+      <c r="N22" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="O22" s="36"/>
-      <c r="P22" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q22" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="O22" s="24"/>
+      <c r="P22" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q22" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="12" t="s">
+      <c r="C23" s="24"/>
+      <c r="D23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G23" s="24" t="s">
+      <c r="G23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H23" s="36" t="s">
+      <c r="H23" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="I23" s="36"/>
-      <c r="J23" s="18" t="s">
+      <c r="I23" s="24"/>
+      <c r="J23" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="K23" s="12" t="s">
+      <c r="K23" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N23" s="55" t="s">
+      <c r="N23" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="O23" s="55"/>
-      <c r="P23" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q23" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="X23" s="28"/>
-      <c r="Y23" s="27"/>
-      <c r="Z23" s="5"/>
-    </row>
-    <row r="24" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O23" s="43"/>
+      <c r="P23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q23" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y23" s="21"/>
+    </row>
+    <row r="24" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="12" t="s">
+      <c r="C24" s="24"/>
+      <c r="D24" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H24" s="38" t="s">
+      <c r="H24" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="38"/>
-      <c r="J24" s="19" t="s">
+      <c r="I24" s="25"/>
+      <c r="J24" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="K24" s="13" t="s">
+      <c r="K24" s="12" t="s">
         <v>53</v>
       </c>
       <c r="M24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N24" s="55" t="s">
+      <c r="N24" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="O24" s="55"/>
-      <c r="P24" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q24" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="V24" s="5"/>
-      <c r="W24" s="28"/>
-      <c r="X24" s="28"/>
-      <c r="Y24" s="27"/>
-      <c r="Z24" s="5"/>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="O24" s="43"/>
+      <c r="P24" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q24" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y24" s="21"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="12" t="s">
+      <c r="C25" s="24"/>
+      <c r="D25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="11" t="s">
         <v>20</v>
       </c>
       <c r="M25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N25" s="55" t="s">
+      <c r="N25" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="O25" s="55"/>
-      <c r="P25" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q25" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O25" s="43"/>
+      <c r="P25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q25" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="12" t="s">
+      <c r="C26" s="24"/>
+      <c r="D26" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>52</v>
       </c>
       <c r="M26" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N26" s="55" t="s">
+      <c r="N26" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="O26" s="55"/>
-      <c r="P26" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q26" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="O26" s="24"/>
+      <c r="P26" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q26" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="12" t="s">
+      <c r="C27" s="24"/>
+      <c r="D27" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H27" s="37" t="s">
+      <c r="H27" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="I27" s="37"/>
+      <c r="I27" s="26"/>
       <c r="J27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K27" s="11" t="s">
+      <c r="K27" s="10" t="s">
         <v>3</v>
       </c>
       <c r="M27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N27" s="55" t="s">
+      <c r="N27" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="O27" s="55"/>
-      <c r="P27" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q27" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="O27" s="24"/>
+      <c r="P27" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q27" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="12" t="s">
+      <c r="C28" s="24"/>
+      <c r="D28" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G28" s="4"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="12"/>
+      <c r="K28" s="11"/>
       <c r="M28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N28" s="55" t="s">
+      <c r="N28" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="O28" s="55"/>
-      <c r="P28" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q28" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="O28" s="24"/>
+      <c r="P28" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q28" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="C29" s="36"/>
-      <c r="D29" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="12" t="s">
+      <c r="C29" s="24"/>
+      <c r="D29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H29" s="36" t="s">
+      <c r="H29" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="I29" s="36"/>
-      <c r="J29" s="17" t="s">
+      <c r="I29" s="24"/>
+      <c r="J29" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K29" s="23" t="s">
+      <c r="K29" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M29" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N29" s="36" t="s">
+      <c r="N29" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="O29" s="36"/>
-      <c r="P29" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q29" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="O29" s="43"/>
+      <c r="P29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q29" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="12" t="s">
+      <c r="C30" s="24"/>
+      <c r="D30" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H30" s="36" t="s">
+      <c r="H30" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="I30" s="36"/>
-      <c r="J30" s="17" t="s">
+      <c r="I30" s="24"/>
+      <c r="J30" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K30" s="23" t="s">
+      <c r="K30" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M30" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N30" s="36" t="s">
+      <c r="N30" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="O30" s="36"/>
-      <c r="P30" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q30" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="W30" s="5"/>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="O30" s="43"/>
+      <c r="P30" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q30" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="C31" s="36"/>
-      <c r="D31" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="12" t="s">
+      <c r="C31" s="24"/>
+      <c r="D31" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G31" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="H31" s="36" t="s">
+      <c r="G31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="I31" s="36"/>
-      <c r="J31" s="17" t="s">
+      <c r="I31" s="24"/>
+      <c r="J31" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K31" s="23" t="s">
+      <c r="K31" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M31" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N31" s="36" t="s">
+      <c r="N31" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="O31" s="36"/>
-      <c r="P31" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q31" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="O31" s="43"/>
+      <c r="P31" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q31" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="12" t="s">
+      <c r="C32" s="24"/>
+      <c r="D32" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H32" s="36" t="s">
+      <c r="H32" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="I32" s="36"/>
-      <c r="J32" s="17" t="s">
+      <c r="I32" s="24"/>
+      <c r="J32" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K32" s="23" t="s">
+      <c r="K32" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M32" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N32" s="36" t="s">
+      <c r="N32" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="O32" s="36"/>
-      <c r="P32" s="14" t="s">
+      <c r="O32" s="24"/>
+      <c r="P32" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q32" s="12" t="s">
+      <c r="Q32" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2335,40 +2304,40 @@
       <c r="A33" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="C33" s="36"/>
-      <c r="D33" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="12" t="s">
+      <c r="C33" s="24"/>
+      <c r="D33" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G33" s="32" t="s">
+      <c r="G33" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H33" s="38" t="s">
+      <c r="H33" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="I33" s="38"/>
-      <c r="J33" s="35" t="s">
+      <c r="I33" s="25"/>
+      <c r="J33" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K33" s="13" t="s">
+      <c r="K33" s="12" t="s">
         <v>53</v>
       </c>
       <c r="M33" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N33" s="36" t="s">
+      <c r="N33" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="O33" s="36"/>
-      <c r="P33" s="14" t="s">
+      <c r="O33" s="24"/>
+      <c r="P33" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q33" s="12" t="s">
+      <c r="Q33" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2376,27 +2345,27 @@
       <c r="A34" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="C34" s="36"/>
-      <c r="D34" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="12" t="s">
+      <c r="C34" s="24"/>
+      <c r="D34" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="11" t="s">
         <v>20</v>
       </c>
       <c r="M34" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N34" s="36" t="s">
+      <c r="N34" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="O34" s="36"/>
-      <c r="P34" s="14" t="s">
+      <c r="O34" s="24"/>
+      <c r="P34" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q34" s="12" t="s">
+      <c r="Q34" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2404,27 +2373,27 @@
       <c r="A35" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="C35" s="36"/>
-      <c r="D35" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="12" t="s">
+      <c r="C35" s="24"/>
+      <c r="D35" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="11" t="s">
         <v>52</v>
       </c>
       <c r="M35" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N35" s="36" t="s">
+      <c r="N35" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="O35" s="36"/>
-      <c r="P35" s="14" t="s">
+      <c r="O35" s="43"/>
+      <c r="P35" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q35" s="12" t="s">
+      <c r="Q35" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2432,40 +2401,40 @@
       <c r="A36" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="C36" s="36"/>
-      <c r="D36" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="12" t="s">
+      <c r="C36" s="24"/>
+      <c r="D36" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H36" s="37" t="s">
+      <c r="H36" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="I36" s="37"/>
-      <c r="J36" s="34" t="s">
+      <c r="I36" s="26"/>
+      <c r="J36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K36" s="11" t="s">
+      <c r="K36" s="10" t="s">
         <v>3</v>
       </c>
       <c r="M36" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N36" s="36" t="s">
+      <c r="N36" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="O36" s="36"/>
-      <c r="P36" s="14" t="s">
+      <c r="O36" s="43"/>
+      <c r="P36" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q36" s="12" t="s">
+      <c r="Q36" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2473,32 +2442,29 @@
       <c r="A37" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="C37" s="36"/>
-      <c r="D37" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="12" t="s">
+      <c r="C37" s="24"/>
+      <c r="D37" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G37" s="4"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="12"/>
+      <c r="K37" s="11"/>
       <c r="M37" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N37" s="36" t="s">
+      <c r="N37" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="O37" s="36"/>
-      <c r="P37" s="14" t="s">
+      <c r="O37" s="43"/>
+      <c r="P37" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q37" s="12" t="s">
+      <c r="Q37" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2506,40 +2472,40 @@
       <c r="A38" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="C38" s="36"/>
-      <c r="D38" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="12" t="s">
+      <c r="C38" s="24"/>
+      <c r="D38" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H38" s="36" t="s">
+      <c r="H38" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="I38" s="36"/>
-      <c r="J38" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="K38" s="12" t="s">
+      <c r="I38" s="24"/>
+      <c r="J38" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="K38" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M38" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N38" s="36" t="s">
+      <c r="N38" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="O38" s="36"/>
-      <c r="P38" s="14" t="s">
+      <c r="O38" s="43"/>
+      <c r="P38" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q38" s="12" t="s">
+      <c r="Q38" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2547,81 +2513,81 @@
       <c r="A39" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="C39" s="36"/>
-      <c r="D39" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="12" t="s">
+      <c r="C39" s="24"/>
+      <c r="D39" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H39" s="36" t="s">
+      <c r="H39" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="I39" s="36"/>
-      <c r="J39" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="K39" s="12" t="s">
+      <c r="I39" s="24"/>
+      <c r="J39" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="K39" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M39" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N39" s="36" t="s">
+      <c r="N39" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="O39" s="36"/>
-      <c r="P39" s="14" t="s">
+      <c r="O39" s="43"/>
+      <c r="P39" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q39" s="12" t="s">
+      <c r="Q39" s="11" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="38" t="s">
+      <c r="B40" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="C40" s="38"/>
-      <c r="D40" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="13" t="s">
+      <c r="C40" s="25"/>
+      <c r="D40" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="12" t="s">
         <v>20</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H40" s="36" t="s">
+      <c r="H40" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="I40" s="36"/>
-      <c r="J40" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="K40" s="12" t="s">
+      <c r="I40" s="24"/>
+      <c r="J40" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="K40" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M40" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N40" s="36" t="s">
+      <c r="N40" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="O40" s="36"/>
-      <c r="P40" s="14" t="s">
+      <c r="O40" s="43"/>
+      <c r="P40" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q40" s="12" t="s">
+      <c r="Q40" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2629,27 +2595,27 @@
       <c r="G41" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H41" s="36" t="s">
+      <c r="H41" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="I41" s="36"/>
-      <c r="J41" s="18" t="s">
+      <c r="I41" s="24"/>
+      <c r="J41" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="K41" s="12" t="s">
+      <c r="K41" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M41" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N41" s="36" t="s">
+      <c r="N41" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="O41" s="36"/>
-      <c r="P41" s="14" t="s">
+      <c r="O41" s="24"/>
+      <c r="P41" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q41" s="12" t="s">
+      <c r="Q41" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2657,27 +2623,27 @@
       <c r="G42" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H42" s="36" t="s">
+      <c r="H42" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="I42" s="36"/>
-      <c r="J42" s="18" t="s">
+      <c r="I42" s="24"/>
+      <c r="J42" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="K42" s="12" t="s">
+      <c r="K42" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M42" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N42" s="36" t="s">
+      <c r="N42" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="O42" s="36"/>
-      <c r="P42" s="14" t="s">
+      <c r="O42" s="24"/>
+      <c r="P42" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q42" s="12" t="s">
+      <c r="Q42" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2685,74 +2651,70 @@
       <c r="A43" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B43" s="37" t="s">
+      <c r="B43" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C43" s="37"/>
-      <c r="D43" s="20" t="s">
+      <c r="C43" s="26"/>
+      <c r="D43" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="E43" s="10" t="s">
         <v>3</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H43" s="36" t="s">
+      <c r="H43" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="I43" s="36"/>
-      <c r="J43" s="14" t="s">
+      <c r="I43" s="24"/>
+      <c r="J43" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="K43" s="12" t="s">
+      <c r="K43" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M43" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N43" s="36" t="s">
+      <c r="N43" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="O43" s="36"/>
-      <c r="P43" s="14" t="s">
+      <c r="O43" s="24"/>
+      <c r="P43" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q43" s="12" t="s">
+      <c r="Q43" s="11" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
-      <c r="B44" s="28"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="5"/>
+      <c r="E44" s="11"/>
       <c r="G44" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H44" s="36" t="s">
+      <c r="H44" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="I44" s="36"/>
-      <c r="J44" s="14" t="s">
+      <c r="I44" s="24"/>
+      <c r="J44" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="K44" s="12" t="s">
+      <c r="K44" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M44" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N44" s="55" t="s">
+      <c r="N44" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="O44" s="55"/>
-      <c r="P44" s="14" t="s">
+      <c r="O44" s="24"/>
+      <c r="P44" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q44" s="12" t="s">
+      <c r="Q44" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2760,41 +2722,40 @@
       <c r="A45" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B45" s="36" t="s">
+      <c r="B45" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C45" s="36"/>
-      <c r="D45" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F45" s="5"/>
-      <c r="G45" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H45" s="38" t="s">
+      <c r="C45" s="24"/>
+      <c r="D45" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H45" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="I45" s="38"/>
-      <c r="J45" s="19" t="s">
+      <c r="I45" s="25"/>
+      <c r="J45" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="K45" s="13" t="s">
+      <c r="K45" s="12" t="s">
         <v>53</v>
       </c>
       <c r="M45" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N45" s="55" t="s">
+      <c r="N45" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="O45" s="55"/>
-      <c r="P45" s="14" t="s">
+      <c r="O45" s="24"/>
+      <c r="P45" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q45" s="12" t="s">
+      <c r="Q45" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2802,28 +2763,27 @@
       <c r="A46" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="36" t="s">
+      <c r="B46" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="36"/>
-      <c r="D46" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F46" s="5"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>53</v>
+      </c>
       <c r="M46" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N46" s="55" t="s">
+      <c r="N46" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="O46" s="55"/>
-      <c r="P46" s="14" t="s">
+      <c r="O46" s="24"/>
+      <c r="P46" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q46" s="12" t="s">
+      <c r="Q46" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2831,27 +2791,27 @@
       <c r="A47" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B47" s="36" t="s">
+      <c r="B47" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="36"/>
-      <c r="D47" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47" s="12" t="s">
+      <c r="C47" s="24"/>
+      <c r="D47" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M47" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N47" s="55" t="s">
+      <c r="N47" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="O47" s="55"/>
-      <c r="P47" s="14" t="s">
+      <c r="O47" s="24"/>
+      <c r="P47" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q47" s="12" t="s">
+      <c r="Q47" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2859,27 +2819,27 @@
       <c r="A48" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B48" s="36" t="s">
+      <c r="B48" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="C48" s="36"/>
-      <c r="D48" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E48" s="12" t="s">
+      <c r="C48" s="24"/>
+      <c r="D48" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M48" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N48" s="55" t="s">
+      <c r="N48" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="O48" s="55"/>
-      <c r="P48" s="14" t="s">
+      <c r="O48" s="24"/>
+      <c r="P48" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q48" s="12" t="s">
+      <c r="Q48" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2887,27 +2847,27 @@
       <c r="A49" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B49" s="36" t="s">
+      <c r="B49" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C49" s="36"/>
-      <c r="D49" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E49" s="12" t="s">
+      <c r="C49" s="24"/>
+      <c r="D49" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M49" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N49" s="55" t="s">
+      <c r="N49" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="O49" s="55"/>
-      <c r="P49" s="14" t="s">
+      <c r="O49" s="24"/>
+      <c r="P49" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q49" s="12" t="s">
+      <c r="Q49" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2915,27 +2875,27 @@
       <c r="A50" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B50" s="36" t="s">
+      <c r="B50" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C50" s="36"/>
-      <c r="D50" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E50" s="12" t="s">
+      <c r="C50" s="24"/>
+      <c r="D50" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M50" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N50" s="55" t="s">
+      <c r="N50" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="O50" s="55"/>
-      <c r="P50" s="18" t="s">
+      <c r="O50" s="24"/>
+      <c r="P50" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="Q50" s="12" t="s">
+      <c r="Q50" s="11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2943,27 +2903,27 @@
       <c r="A51" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B51" s="36" t="s">
+      <c r="B51" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C51" s="36"/>
-      <c r="D51" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E51" s="12" t="s">
+      <c r="C51" s="24"/>
+      <c r="D51" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M51" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N51" s="55" t="s">
+      <c r="N51" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="O51" s="55"/>
-      <c r="P51" s="18" t="s">
+      <c r="O51" s="24"/>
+      <c r="P51" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="Q51" s="12" t="s">
+      <c r="Q51" s="11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2971,27 +2931,27 @@
       <c r="A52" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B52" s="36" t="s">
+      <c r="B52" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C52" s="36"/>
-      <c r="D52" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E52" s="12" t="s">
+      <c r="C52" s="24"/>
+      <c r="D52" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M52" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N52" s="55" t="s">
+      <c r="N52" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="O52" s="55"/>
-      <c r="P52" s="18" t="s">
+      <c r="O52" s="24"/>
+      <c r="P52" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="Q52" s="12" t="s">
+      <c r="Q52" s="11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2999,27 +2959,27 @@
       <c r="A53" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B53" s="36" t="s">
+      <c r="B53" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="36"/>
-      <c r="D53" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E53" s="12" t="s">
+      <c r="C53" s="24"/>
+      <c r="D53" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M53" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N53" s="55" t="s">
+      <c r="N53" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="O53" s="55"/>
-      <c r="P53" s="18" t="s">
+      <c r="O53" s="24"/>
+      <c r="P53" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="Q53" s="12" t="s">
+      <c r="Q53" s="11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3027,27 +2987,27 @@
       <c r="A54" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B54" s="36" t="s">
+      <c r="B54" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C54" s="36"/>
-      <c r="D54" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54" s="12" t="s">
+      <c r="C54" s="24"/>
+      <c r="D54" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M54" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N54" s="55" t="s">
+      <c r="N54" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="O54" s="55"/>
-      <c r="P54" s="18" t="s">
+      <c r="O54" s="24"/>
+      <c r="P54" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="Q54" s="12" t="s">
+      <c r="Q54" s="11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3055,27 +3015,27 @@
       <c r="A55" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B55" s="36" t="s">
+      <c r="B55" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C55" s="36"/>
-      <c r="D55" s="17" t="s">
+      <c r="C55" s="24"/>
+      <c r="D55" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E55" s="12" t="s">
+      <c r="E55" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="M55" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N55" s="56" t="s">
+      <c r="M55" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N55" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="O55" s="56"/>
-      <c r="P55" s="19" t="s">
+      <c r="O55" s="25"/>
+      <c r="P55" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="Q55" s="13" t="s">
+      <c r="Q55" s="12" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3083,14 +3043,14 @@
       <c r="A56" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B56" s="36" t="s">
+      <c r="B56" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C56" s="36"/>
-      <c r="D56" s="18" t="s">
+      <c r="C56" s="24"/>
+      <c r="D56" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E56" s="12" t="s">
+      <c r="E56" s="11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3098,14 +3058,14 @@
       <c r="A57" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B57" s="36" t="s">
+      <c r="B57" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C57" s="36"/>
-      <c r="D57" s="18" t="s">
+      <c r="C57" s="24"/>
+      <c r="D57" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E57" s="12" t="s">
+      <c r="E57" s="11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3113,62 +3073,59 @@
       <c r="A58" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B58" s="36" t="s">
+      <c r="B58" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C58" s="36"/>
-      <c r="D58" s="18" t="s">
+      <c r="C58" s="24"/>
+      <c r="D58" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E58" s="12" t="s">
+      <c r="E58" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M58" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N58" s="37" t="s">
+      <c r="N58" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="O58" s="37"/>
+      <c r="O58" s="26"/>
       <c r="P58" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="Q58" s="11" t="s">
+      <c r="Q58" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="8" t="s">
+      <c r="A59" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B59" s="38" t="s">
+      <c r="B59" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C59" s="38"/>
-      <c r="D59" s="19" t="s">
+      <c r="C59" s="25"/>
+      <c r="D59" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E59" s="13" t="s">
+      <c r="E59" s="12" t="s">
         <v>53</v>
       </c>
       <c r="M59" s="4"/>
-      <c r="N59" s="5"/>
-      <c r="O59" s="5"/>
-      <c r="P59" s="5"/>
-      <c r="Q59" s="12"/>
+      <c r="Q59" s="11"/>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="M60" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N60" s="36" t="s">
+      <c r="N60" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="O60" s="36"/>
-      <c r="P60" s="17" t="s">
+      <c r="O60" s="24"/>
+      <c r="P60" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="Q60" s="12" t="s">
+      <c r="Q60" s="11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3176,14 +3133,14 @@
       <c r="M61" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N61" s="36" t="s">
+      <c r="N61" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="O61" s="36"/>
-      <c r="P61" s="17" t="s">
+      <c r="O61" s="24"/>
+      <c r="P61" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="Q61" s="12" t="s">
+      <c r="Q61" s="11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3191,47 +3148,44 @@
       <c r="A62" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B62" s="39" t="s">
+      <c r="B62" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C62" s="39"/>
-      <c r="D62" s="20" t="s">
+      <c r="C62" s="27"/>
+      <c r="D62" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E62" s="11" t="s">
+      <c r="E62" s="10" t="s">
         <v>3</v>
       </c>
       <c r="M62" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N62" s="36" t="s">
+      <c r="N62" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="O62" s="36"/>
-      <c r="P62" s="17" t="s">
+      <c r="O62" s="24"/>
+      <c r="P62" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="Q62" s="12" t="s">
+      <c r="Q62" s="11" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="12"/>
+      <c r="E63" s="11"/>
       <c r="M63" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N63" s="36" t="s">
+      <c r="N63" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="O63" s="36"/>
-      <c r="P63" s="17" t="s">
+      <c r="O63" s="24"/>
+      <c r="P63" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="Q63" s="12" t="s">
+      <c r="Q63" s="11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3239,27 +3193,27 @@
       <c r="A64" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B64" s="36" t="s">
+      <c r="B64" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C64" s="36"/>
-      <c r="D64" s="17" t="s">
+      <c r="C64" s="24"/>
+      <c r="D64" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E64" s="12" t="s">
+      <c r="E64" s="11" t="s">
         <v>24</v>
       </c>
       <c r="M64" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N64" s="36" t="s">
+      <c r="N64" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="O64" s="36"/>
-      <c r="P64" s="17" t="s">
+      <c r="O64" s="24"/>
+      <c r="P64" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="Q64" s="12" t="s">
+      <c r="Q64" s="11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3267,27 +3221,27 @@
       <c r="A65" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B65" s="36" t="s">
+      <c r="B65" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C65" s="36"/>
-      <c r="D65" s="17" t="s">
+      <c r="C65" s="24"/>
+      <c r="D65" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E65" s="12" t="s">
+      <c r="E65" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="M65" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N65" s="38" t="s">
+      <c r="M65" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N65" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="O65" s="38"/>
-      <c r="P65" s="35" t="s">
+      <c r="O65" s="25"/>
+      <c r="P65" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="Q65" s="13" t="s">
+      <c r="Q65" s="12" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3295,14 +3249,14 @@
       <c r="A66" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B66" s="36" t="s">
+      <c r="B66" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C66" s="36"/>
-      <c r="D66" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E66" s="12" t="s">
+      <c r="C66" s="24"/>
+      <c r="D66" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" s="11" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3310,14 +3264,14 @@
       <c r="A67" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B67" s="36" t="s">
+      <c r="B67" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="C67" s="36"/>
-      <c r="D67" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E67" s="12" t="s">
+      <c r="C67" s="24"/>
+      <c r="D67" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" s="11" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3325,14 +3279,14 @@
       <c r="A68" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B68" s="36" t="s">
+      <c r="B68" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C68" s="36"/>
-      <c r="D68" s="17" t="s">
+      <c r="C68" s="24"/>
+      <c r="D68" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E68" s="12" t="s">
+      <c r="E68" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3340,454 +3294,242 @@
       <c r="A69" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B69" s="36" t="s">
+      <c r="B69" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C69" s="36"/>
-      <c r="D69" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E69" s="12" t="s">
+      <c r="C69" s="24"/>
+      <c r="D69" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" s="11" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="8" t="s">
+      <c r="A70" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B70" s="38" t="s">
+      <c r="B70" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C70" s="38"/>
-      <c r="D70" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E70" s="13" t="s">
+      <c r="C70" s="25"/>
+      <c r="D70" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A80" s="29"/>
-      <c r="B80" s="30"/>
-      <c r="C80" s="30"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="22"/>
-      <c r="G80" s="22"/>
-      <c r="H80" s="30"/>
-      <c r="I80" s="30"/>
-      <c r="J80" s="22"/>
-      <c r="K80" s="22"/>
-      <c r="M80" s="22"/>
-      <c r="N80" s="30"/>
-      <c r="O80" s="30"/>
-      <c r="P80" s="22"/>
-      <c r="Q80" s="22"/>
-    </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A81" s="22"/>
-      <c r="B81" s="22"/>
-      <c r="C81" s="22"/>
-      <c r="D81" s="22"/>
-      <c r="E81" s="22"/>
-      <c r="G81" s="22"/>
-      <c r="H81" s="22"/>
-      <c r="I81" s="22"/>
-      <c r="J81" s="22"/>
-      <c r="K81" s="22"/>
-      <c r="M81" s="22"/>
-      <c r="N81" s="22"/>
-      <c r="O81" s="22"/>
-      <c r="P81" s="22"/>
-      <c r="Q81" s="22"/>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A82" s="22"/>
-      <c r="B82" s="29"/>
-      <c r="C82" s="29"/>
-      <c r="D82" s="27"/>
-      <c r="E82" s="22"/>
-      <c r="G82" s="22"/>
-      <c r="H82" s="29"/>
-      <c r="I82" s="29"/>
-      <c r="J82" s="27"/>
-      <c r="K82" s="22"/>
-      <c r="M82" s="22"/>
-      <c r="N82" s="29"/>
-      <c r="O82" s="29"/>
-      <c r="P82" s="27"/>
-      <c r="Q82" s="22"/>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A83" s="22"/>
-      <c r="B83" s="29"/>
-      <c r="C83" s="29"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="22"/>
-      <c r="G83" s="22"/>
-      <c r="H83" s="29"/>
-      <c r="I83" s="29"/>
-      <c r="J83" s="27"/>
-      <c r="K83" s="22"/>
-      <c r="M83" s="22"/>
-      <c r="N83" s="29"/>
-      <c r="O83" s="29"/>
-      <c r="P83" s="27"/>
-      <c r="Q83" s="22"/>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A84" s="22"/>
-      <c r="B84" s="29"/>
-      <c r="C84" s="29"/>
-      <c r="D84" s="27"/>
-      <c r="E84" s="22"/>
-      <c r="G84" s="22"/>
-      <c r="H84" s="29"/>
-      <c r="I84" s="29"/>
-      <c r="J84" s="27"/>
-      <c r="K84" s="22"/>
-      <c r="M84" s="22"/>
-      <c r="N84" s="29"/>
-      <c r="O84" s="29"/>
-      <c r="P84" s="27"/>
-      <c r="Q84" s="22"/>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A85" s="22"/>
-      <c r="B85" s="29"/>
-      <c r="C85" s="29"/>
-      <c r="D85" s="27"/>
-      <c r="E85" s="22"/>
-      <c r="G85" s="22"/>
-      <c r="H85" s="29"/>
-      <c r="I85" s="29"/>
-      <c r="J85" s="31"/>
-      <c r="K85" s="22"/>
-      <c r="M85" s="22"/>
-      <c r="N85" s="29"/>
-      <c r="O85" s="29"/>
-      <c r="P85" s="27"/>
-      <c r="Q85" s="22"/>
-    </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A86" s="22"/>
-      <c r="B86" s="29"/>
-      <c r="C86" s="29"/>
-      <c r="D86" s="27"/>
-      <c r="E86" s="22"/>
-      <c r="G86" s="22"/>
-      <c r="H86" s="29"/>
-      <c r="I86" s="29"/>
-      <c r="J86" s="27"/>
-      <c r="K86" s="22"/>
-      <c r="M86" s="22"/>
-      <c r="N86" s="29"/>
-      <c r="O86" s="29"/>
-      <c r="P86" s="27"/>
-      <c r="Q86" s="22"/>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A87" s="22"/>
-      <c r="B87" s="29"/>
-      <c r="C87" s="29"/>
-      <c r="D87" s="27"/>
-      <c r="E87" s="22"/>
-      <c r="G87" s="22"/>
-      <c r="H87" s="29"/>
-      <c r="I87" s="29"/>
-      <c r="J87" s="27"/>
-      <c r="K87" s="22"/>
-      <c r="M87" s="22"/>
-      <c r="N87" s="29"/>
-      <c r="O87" s="29"/>
-      <c r="P87" s="27"/>
-      <c r="Q87" s="22"/>
-    </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A88" s="22"/>
-      <c r="B88" s="29"/>
-      <c r="C88" s="29"/>
-      <c r="D88" s="27"/>
-      <c r="E88" s="22"/>
-      <c r="G88" s="22"/>
-      <c r="H88" s="29"/>
-      <c r="I88" s="29"/>
-      <c r="J88" s="27"/>
-      <c r="K88" s="22"/>
-      <c r="M88" s="22"/>
-      <c r="N88" s="29"/>
-      <c r="O88" s="29"/>
-      <c r="P88" s="27"/>
-      <c r="Q88" s="22"/>
-    </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A89" s="22"/>
-      <c r="B89" s="29"/>
-      <c r="C89" s="29"/>
-      <c r="D89" s="27"/>
-      <c r="E89" s="22"/>
-      <c r="G89" s="22"/>
-      <c r="H89" s="29"/>
-      <c r="I89" s="29"/>
-      <c r="J89" s="27"/>
-      <c r="K89" s="22"/>
-      <c r="M89" s="22"/>
-      <c r="N89" s="29"/>
-      <c r="O89" s="29"/>
-      <c r="P89" s="27"/>
-      <c r="Q89" s="22"/>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A90" s="22"/>
-      <c r="B90" s="29"/>
-      <c r="C90" s="29"/>
-      <c r="D90" s="27"/>
-      <c r="E90" s="22"/>
-      <c r="G90" s="22"/>
-      <c r="H90" s="29"/>
-      <c r="I90" s="29"/>
-      <c r="J90" s="27"/>
-      <c r="K90" s="22"/>
-      <c r="M90" s="22"/>
-      <c r="N90" s="29"/>
-      <c r="O90" s="29"/>
-      <c r="P90" s="27"/>
-      <c r="Q90" s="22"/>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A91" s="22"/>
-      <c r="B91" s="29"/>
-      <c r="C91" s="29"/>
-      <c r="D91" s="27"/>
-      <c r="E91" s="22"/>
-      <c r="G91" s="22"/>
-      <c r="H91" s="29"/>
-      <c r="I91" s="29"/>
-      <c r="J91" s="27"/>
-      <c r="K91" s="22"/>
-      <c r="M91" s="22"/>
-      <c r="N91" s="29"/>
-      <c r="O91" s="29"/>
-      <c r="P91" s="27"/>
-      <c r="Q91" s="22"/>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A92" s="22"/>
-      <c r="B92" s="29"/>
-      <c r="C92" s="29"/>
-      <c r="D92" s="27"/>
-      <c r="E92" s="22"/>
-      <c r="G92" s="22"/>
-      <c r="H92" s="29"/>
-      <c r="I92" s="29"/>
-      <c r="J92" s="27"/>
-      <c r="K92" s="22"/>
-      <c r="M92" s="22"/>
-      <c r="N92" s="29"/>
-      <c r="O92" s="29"/>
-      <c r="P92" s="27"/>
-      <c r="Q92" s="22"/>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A93" s="22"/>
-      <c r="B93" s="22"/>
-      <c r="C93" s="22"/>
-      <c r="D93" s="22"/>
-      <c r="E93" s="22"/>
-      <c r="G93" s="22"/>
-      <c r="H93" s="29"/>
-      <c r="I93" s="29"/>
-      <c r="J93" s="27"/>
-      <c r="K93" s="22"/>
-      <c r="M93" s="22"/>
-      <c r="N93" s="29"/>
-      <c r="O93" s="29"/>
-      <c r="P93" s="27"/>
-      <c r="Q93" s="22"/>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A94" s="22"/>
-      <c r="B94" s="22"/>
-      <c r="C94" s="22"/>
-      <c r="D94" s="22"/>
-      <c r="E94" s="22"/>
-      <c r="G94" s="22"/>
-      <c r="H94" s="29"/>
-      <c r="I94" s="29"/>
-      <c r="J94" s="27"/>
-      <c r="K94" s="22"/>
-      <c r="M94" s="22"/>
-      <c r="N94" s="29"/>
-      <c r="O94" s="29"/>
-      <c r="P94" s="27"/>
-      <c r="Q94" s="22"/>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A95" s="22"/>
-      <c r="B95" s="30"/>
-      <c r="C95" s="30"/>
-      <c r="D95" s="22"/>
-      <c r="E95" s="22"/>
-      <c r="M95" s="22"/>
-      <c r="N95" s="29"/>
-      <c r="O95" s="29"/>
-      <c r="P95" s="27"/>
-      <c r="Q95" s="22"/>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A96" s="22"/>
-      <c r="B96" s="22"/>
-      <c r="C96" s="22"/>
-      <c r="D96" s="22"/>
-      <c r="E96" s="22"/>
-      <c r="M96" s="22"/>
-      <c r="N96" s="29"/>
-      <c r="O96" s="29"/>
-      <c r="P96" s="27"/>
-      <c r="Q96" s="22"/>
-    </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A97" s="22"/>
-      <c r="B97" s="29"/>
-      <c r="C97" s="29"/>
-      <c r="D97" s="27"/>
-      <c r="E97" s="22"/>
-      <c r="M97" s="22"/>
-      <c r="N97" s="29"/>
-      <c r="O97" s="29"/>
-      <c r="P97" s="27"/>
-      <c r="Q97" s="22"/>
-    </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A98" s="22"/>
-      <c r="B98" s="29"/>
-      <c r="C98" s="29"/>
-      <c r="D98" s="27"/>
-      <c r="E98" s="22"/>
-    </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A99" s="22"/>
-      <c r="B99" s="29"/>
-      <c r="C99" s="29"/>
-      <c r="D99" s="27"/>
-      <c r="E99" s="22"/>
-      <c r="F99" s="5"/>
-      <c r="G99" s="5"/>
-      <c r="H99" s="5"/>
-      <c r="I99" s="5"/>
-      <c r="J99" s="5"/>
-      <c r="K99" s="5"/>
-    </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A100" s="22"/>
-      <c r="B100" s="29"/>
-      <c r="C100" s="29"/>
-      <c r="D100" s="27"/>
-      <c r="E100" s="22"/>
-      <c r="F100" s="5"/>
-      <c r="G100" s="5"/>
-      <c r="H100" s="5"/>
-      <c r="I100" s="5"/>
-      <c r="J100" s="5"/>
-      <c r="K100" s="5"/>
-    </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A101" s="22"/>
-      <c r="B101" s="29"/>
-      <c r="C101" s="29"/>
-      <c r="D101" s="27"/>
-      <c r="E101" s="22"/>
-      <c r="F101" s="5"/>
-      <c r="G101" s="5"/>
-      <c r="H101" s="5"/>
-      <c r="I101" s="5"/>
-      <c r="J101" s="5"/>
-      <c r="K101" s="5"/>
-    </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A102" s="22"/>
-      <c r="B102" s="29"/>
-      <c r="C102" s="29"/>
-      <c r="D102" s="27"/>
-      <c r="E102" s="22"/>
-      <c r="F102" s="5"/>
-      <c r="G102" s="5"/>
-      <c r="H102" s="5"/>
-      <c r="I102" s="5"/>
-      <c r="J102" s="5"/>
-      <c r="K102" s="5"/>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A103" s="22"/>
-      <c r="B103" s="29"/>
-      <c r="C103" s="29"/>
-      <c r="D103" s="27"/>
-      <c r="E103" s="22"/>
-      <c r="F103" s="5"/>
-      <c r="G103" s="5"/>
-      <c r="H103" s="28"/>
-      <c r="I103" s="28"/>
-      <c r="J103" s="5"/>
-      <c r="K103" s="5"/>
-    </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="E104" s="5"/>
-      <c r="F104" s="5"/>
-      <c r="G104" s="5"/>
-      <c r="H104" s="5"/>
-      <c r="I104" s="5"/>
-      <c r="J104" s="5"/>
-      <c r="K104" s="5"/>
-    </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="E105" s="5"/>
-      <c r="F105" s="5"/>
-      <c r="G105" s="5"/>
-      <c r="H105" s="33"/>
-      <c r="I105" s="33"/>
-      <c r="J105" s="5"/>
-      <c r="K105" s="5"/>
-    </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="E106" s="5"/>
-      <c r="F106" s="5"/>
-      <c r="G106" s="5"/>
-      <c r="H106" s="5"/>
-      <c r="I106" s="5"/>
-      <c r="J106" s="5"/>
-      <c r="K106" s="5"/>
-    </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="E107" s="5"/>
-      <c r="F107" s="5"/>
-      <c r="G107" s="5"/>
-      <c r="H107" s="5"/>
-      <c r="I107" s="5"/>
-      <c r="J107" s="5"/>
-      <c r="K107" s="5"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="21"/>
+      <c r="H80" s="21"/>
+      <c r="I80" s="21"/>
+      <c r="N80" s="21"/>
+      <c r="O80" s="21"/>
+    </row>
+    <row r="82" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D82" s="21"/>
+      <c r="J82" s="21"/>
+      <c r="P82" s="21"/>
+    </row>
+    <row r="83" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D83" s="21"/>
+      <c r="J83" s="21"/>
+      <c r="P83" s="21"/>
+    </row>
+    <row r="84" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D84" s="21"/>
+      <c r="J84" s="21"/>
+      <c r="P84" s="21"/>
+    </row>
+    <row r="85" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D85" s="21"/>
+      <c r="J85" s="22"/>
+      <c r="P85" s="21"/>
+    </row>
+    <row r="86" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D86" s="21"/>
+      <c r="J86" s="21"/>
+      <c r="P86" s="21"/>
+    </row>
+    <row r="87" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D87" s="21"/>
+      <c r="J87" s="21"/>
+      <c r="P87" s="21"/>
+    </row>
+    <row r="88" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D88" s="21"/>
+      <c r="J88" s="21"/>
+      <c r="P88" s="21"/>
+    </row>
+    <row r="89" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D89" s="21"/>
+      <c r="J89" s="21"/>
+      <c r="P89" s="21"/>
+    </row>
+    <row r="90" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D90" s="21"/>
+      <c r="J90" s="21"/>
+      <c r="P90" s="21"/>
+    </row>
+    <row r="91" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D91" s="21"/>
+      <c r="J91" s="21"/>
+      <c r="P91" s="21"/>
+    </row>
+    <row r="92" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D92" s="21"/>
+      <c r="J92" s="21"/>
+      <c r="P92" s="21"/>
+    </row>
+    <row r="93" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="J93" s="21"/>
+      <c r="P93" s="21"/>
+    </row>
+    <row r="94" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="J94" s="21"/>
+      <c r="P94" s="21"/>
+    </row>
+    <row r="95" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B95" s="21"/>
+      <c r="C95" s="21"/>
+      <c r="P95" s="21"/>
+    </row>
+    <row r="96" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P96" s="21"/>
+    </row>
+    <row r="97" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D97" s="21"/>
+      <c r="P97" s="21"/>
+    </row>
+    <row r="98" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D98" s="21"/>
+    </row>
+    <row r="99" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D99" s="21"/>
+    </row>
+    <row r="100" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D100" s="21"/>
+    </row>
+    <row r="101" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D101" s="21"/>
+    </row>
+    <row r="102" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D102" s="21"/>
+    </row>
+    <row r="103" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D103" s="21"/>
+    </row>
+    <row r="105" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="H105" s="21"/>
+      <c r="I105" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="151">
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="N40:O40"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="N42:O42"/>
-    <mergeCell ref="N43:O43"/>
-    <mergeCell ref="N54:O54"/>
-    <mergeCell ref="N55:O55"/>
-    <mergeCell ref="N49:O49"/>
-    <mergeCell ref="N50:O50"/>
-    <mergeCell ref="N51:O51"/>
-    <mergeCell ref="N52:O52"/>
-    <mergeCell ref="N53:O53"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="N46:O46"/>
-    <mergeCell ref="N47:O47"/>
-    <mergeCell ref="N48:O48"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="T9:V9"/>
+    <mergeCell ref="T8:V8"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="N65:O65"/>
+    <mergeCell ref="N64:O64"/>
+    <mergeCell ref="N63:O63"/>
+    <mergeCell ref="N62:O62"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="N60:O60"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="B39:C39"/>
@@ -3812,112 +3554,30 @@
     <mergeCell ref="B52:C52"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="N58:O58"/>
-    <mergeCell ref="N65:O65"/>
-    <mergeCell ref="N64:O64"/>
-    <mergeCell ref="N63:O63"/>
-    <mergeCell ref="N62:O62"/>
-    <mergeCell ref="N61:O61"/>
-    <mergeCell ref="N60:O60"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="T9:V9"/>
-    <mergeCell ref="T8:V8"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="A1:D3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="N42:O42"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="N54:O54"/>
+    <mergeCell ref="N55:O55"/>
+    <mergeCell ref="N49:O49"/>
+    <mergeCell ref="N50:O50"/>
+    <mergeCell ref="N51:O51"/>
+    <mergeCell ref="N52:O52"/>
+    <mergeCell ref="N53:O53"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="N48:O48"/>
     <mergeCell ref="H40:I40"/>
     <mergeCell ref="H41:I41"/>
     <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H45:I45"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>